<commit_message>
nova base de dados sem auth pass
</commit_message>
<xml_diff>
--- a/netflix.xlsx
+++ b/netflix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa51d375fc037b21/Documentos/CDADOS/cdados-netflix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_EF141E81000AE636A5D03D3DA9AD678B21B02DA5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{03666ED2-5F2C-4D29-BE6C-78E7F370C001}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_EF141E81000AE636A5C0B1595D4C42D320B02DCA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{40DC080D-2FB5-4522-AAE4-B96E64D8BF4C}"/>
   <bookViews>
-    <workbookView xWindow="912" yWindow="-108" windowWidth="22236" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="912" yWindow="-108" windowWidth="22236" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,678 +21,473 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="502">
   <si>
     <t>Treinamento</t>
   </si>
   <si>
-    <t>@dudagatakk @netflixbrasil obrigada netflix!!! vc me dxa mto feliz com todo esse carinho</t>
-  </si>
-  <si>
-    <t>@semspoiler_ @planetalivrosbr será que eles vão tirar esse selo da netflix em alguma edição?</t>
+    <t>@zanchettagui :(
+ah no show dele do netflix ele chamou especialistas de humanas pra falar quando ele tava falando de humanas vai</t>
+  </si>
+  <si>
+    <t>jojo vai chegar na netflix mês q vem, será q eu finalmente vou começar a assistir e virar jojofag?</t>
+  </si>
+  <si>
+    <t>com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>estou rachando o bico com o filme cabras da peste, tem na netflix</t>
+  </si>
+  <si>
+    <t>@twolana9 netflix 
+forças complex</t>
+  </si>
+  <si>
+    <t>@du_senna21 que ódio da netflix!</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa que a alina é a maior do mundo ninguém está acima dela</t>
+  </si>
+  <si>
+    <t>fui testar o aleatório da netflix e eles me mandaram diretamente amanhecer q isso um filme</t>
+  </si>
+  <si>
+    <t>@foikklore ela disse que tava só esperando a confirmação da netflix korea</t>
+  </si>
+  <si>
+    <t>não acredito que a netflix tirou lion do catálogo não</t>
+  </si>
+  <si>
+    <t>eu quase que faço unsubscribe à netflix quando carrego numa série para ver e aparece o “trailer” cheio de spoilers... q ódio https://t.co/zbea99ljod</t>
+  </si>
+  <si>
+    <t>@fabifbbr com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>aí tava vendo "professor iglesias(netflix)" e um aluno preto dele disse assim:
+"vc sabe de como é dificil ser considerado um homem preto muito bonito hoje em dia? o michael b jordan elevou a barra à um nível inalcançável." https://t.co/gdq6llfm07</t>
+  </si>
+  <si>
+    <t>@nikofscars não me lembra teve oq? duas fotos deles? nossa netflix pfvr nos alimente um pouquinho...</t>
+  </si>
+  <si>
+    <t>@_otakusbr @tlagartin vai me passar a senha da netflix ou não</t>
+  </si>
+  <si>
+    <t>essa foto da perrie me lembrou next in fashion
+netflix, eu nunca vou te perdoar por cancelar o melhor reality de moda https://t.co/c1fyard6ny</t>
+  </si>
+  <si>
+    <t>agora que tenho o amazon prime, nunca mais assisti netflix kkk é muito melhor</t>
+  </si>
+  <si>
+    <t>já arrumei a casa toda, pia pela netflix.😴</t>
+  </si>
+  <si>
+    <t>⚠️⚠️tentativa de interação⚠️⚠️
+oq tem no seu continuar assistindo na netflix? 
+me:
+não gostei de ginny e georgia 
+bridgerton não tá sendo oq eu esperava 
+tô revendo the society 
+comecei dcd ontem e não terminei https://t.co/br3kvkgdzt</t>
+  </si>
+  <si>
+    <t>o garoto falou assim pra mim: mas tu assiste netflix mesmo? ou é igual aquelas pessoas que finge? ai eu: não entendi, ele: as que falam que assiste mas é só pra transar (?????) o que é jesus?? o que eu fiz pra merecer machos assim</t>
+  </si>
+  <si>
+    <t>por influência do @budejopodcast  acabei de assistir cabras da peste , na netflix, com @edcoisativo . o filme tá excelente!!! um alívio cômico no meio desse caos. recomendo demais</t>
+  </si>
+  <si>
+    <t>acabei de ver que a netflix criou outra série de patinação no gelo invés de ter renovado spinning out</t>
+  </si>
+  <si>
+    <t>ela gosta de netflix playstation 4, mas só eu sei como ela joga no quarto</t>
+  </si>
+  <si>
+    <t>impressionante como a netflix caga em um todos finais que faz, o recepcionista é um baita filma, mas o final é cagado</t>
+  </si>
+  <si>
+    <t>apenas os conteúdos exclusivos, como programas, séries e filmes exigem uma assinatura paga. 
+eu acho essa estratégia muito inteligente, e em terras de globoplay e netflix, seria uma boa!</t>
+  </si>
+  <si>
+    <t>@jmsubmin @floraskata manoooooo que vergonha sério pq eu absolutamente amo os dois kkkkkkkkk o steve é inclusive minha fotinha no netflix, sla acho que faz tanto tempo que eu vi qualquer coisa relacionado a  st que eu esqueci completamente</t>
+  </si>
+  <si>
+    <t>tanto anime bom pra botar no catálogo e a netflix vai botar jojo</t>
+  </si>
+  <si>
+    <t>novo conceito de romance da netflix: rolê na funerária, ouvir musiquinha deitados dentro de um caixão 
+gostei vou aderir</t>
+  </si>
+  <si>
+    <t>finalmente algo bom na netflix https://t.co/glywym0gcg</t>
+  </si>
+  <si>
+    <t>se depender da netflix br ela continua sendo só nossa https://t.co/0bpmeyysj1 https://t.co/d04ipkp31o</t>
+  </si>
+  <si>
+    <t>@vicionerd16 
+agora que jojo vai inteiro pra netflix
+será que sai dublagem? https://t.co/hxfecg1llk</t>
+  </si>
+  <si>
+    <t>@itsfelixwot deity🥵✨#ginnyandgeorgia #marcus 
+@netflix https://t.co/qxwhhluqou</t>
+  </si>
+  <si>
+    <t>seu futuro na netflix? se isso é um sonho, eu não quero acordar 😭😍 https://t.co/uwxlvhkq2q</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa q ela é a rainha</t>
+  </si>
+  <si>
+    <t>jojo's vai lançar na netflix no dia do meu aniversário 🙏</t>
+  </si>
+  <si>
+    <t>eu só queria shameless us na porra da netflix ou pelo menos em algum outro canal de streaming pq mds cansado de tentar conseguir baixar isso</t>
+  </si>
+  <si>
+    <t>@_animese obrigado netflix, vai ser mais fácil eu por minha mãe pra assistir cmg e com meu irmão 🤝🤝😂</t>
+  </si>
+  <si>
+    <t>e fomos de trabalhar mais que a netflix 
+sky rojo tomorrow</t>
+  </si>
+  <si>
+    <t>tenho maior raiva da netflix porque tem conteúdo de cursed que nem foi ai ar e eles esqueceram disso né @netflixbrasil</t>
+  </si>
+  <si>
+    <t>@janinha_criis @nnsafl @hauntingbrasil @hauntingmidias @amaldicaobr é uma série da netflix, a maldição da residência hill, é muito boa, recomendo demais</t>
+  </si>
+  <si>
+    <t>“estou assistindo a programas infantis com ela(khai) na tv e na netflix, aprendendo versos infantis, passeando com ela e cantando para ela, é um ritmo de vida muito diferente, mas tem sido muito fácil de ajustar e isso é o mais surpreendente”</t>
+  </si>
+  <si>
+    <t>oito séries espanholas para ver na netflix (além d’ a casa de papel) https://t.co/ghidm56vnw https://t.co/qas1sdwuor</t>
+  </si>
+  <si>
+    <t>comédia policial à brasileira, cabras da peste estreia na netflix. #ndmais https://t.co/yskcqxphev</t>
+  </si>
+  <si>
+    <t>vi o filme na netflix das bruxas silenciadas e quero entender o final, elas morreram? elas conseguiram "voar"? elas eram realmente bruxas? o filme em si é perfeito mas eu sou ruim em interpretação</t>
+  </si>
+  <si>
+    <t>pra quem não me conhece eu sou a netflix de aruanda kkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>era pra rir netflix? pq eu tô chorando https://t.co/ik7xb93gnw</t>
+  </si>
+  <si>
+    <t>@netflixbrasil vou maratonar essa em um dia netflix</t>
+  </si>
+  <si>
+    <t>@bhtgds já viu sem maturidade pra isso? animação boa
+original netflix</t>
+  </si>
+  <si>
+    <t>@gabister__ pra que netflix? tu pode ver "uma beleza fantástica" em qualquer espelho por aí https://t.co/wjpmivmwnt</t>
+  </si>
+  <si>
+    <t>sapatões vejam esse filme que entrou hoje na netflix. por trás da inocência https://t.co/rpornefwnc</t>
+  </si>
+  <si>
+    <t>@miguelrude @muringa77 primer é clássico, pra derreter o cérebro.
+the void é aquele que tem uma vibe  de lovecraft, né? já vi sim.
+a vastidão da noite ainda não vi, mas muita gente falou bem, fiquei curioso.
+já viu o ritual? esse tem na netflix.</t>
+  </si>
+  <si>
+    <t>@wfoxmoon deve ser amg pq meu deus kkkkkkkk
+fora q a netflix tb vem com uns nomes nada ver</t>
+  </si>
+  <si>
+    <t>será que a netflix vai lançar incon da série de grisha???? aaaaaaaansiosaaaaaaa</t>
   </si>
   <si>
     <t>@allantelesm @promodelivro se tivessem falado q era só uma série de fada teria sido aceitável, mas chamar esse treco horroroso de série das winx..... uma ofensa a nossa infância 
 netflix nunca pecou tanto</t>
   </si>
   <si>
-    <t>quinta -feira cheio de trabalho,  tô  cansada, viu??
-estou em home office celestial...eu e a netflix!! o céu d verdade  é  na nossa casa, isso não  tem preço!!  ❤🙏 https://t.co/rzolvc1kff</t>
-  </si>
-  <si>
-    <t>amanda deixou forte com a conta da netflix ❤</t>
-  </si>
-  <si>
-    <t>@netflixbrasil netflix a seleção é real ou lenda urbana?</t>
-  </si>
-  <si>
-    <t>eu fui ver minha lista da netflix e so tem dorama e anime</t>
-  </si>
-  <si>
-    <t>era só alguém pra emprestando uma conta da netflix 🤧</t>
-  </si>
-  <si>
-    <t>fui testar o aleatório da netflix e eles me mandaram diretamente amanhecer q isso um filme</t>
-  </si>
-  <si>
-    <t>@_virso_ o quarto é tenku shinpan, tem no netflix e é bem bão</t>
-  </si>
-  <si>
-    <t>@_animese meu deus jojo na netflix eu precisa disso</t>
-  </si>
-  <si>
-    <t>cadê a 4 temporada de elite dona netflix
-#elite4</t>
-  </si>
-  <si>
-    <t>o caleb com quase 20 anos vei kkkkkkkkkkkkkk netflix agiliza ai https://t.co/7aiop81jhs</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. não
-2. oficialmente nenhuma, escondido da minha mãe 3
-3. todos
-4. sei lá
-5. desapegada
-6. jamais
-7. já fui
-8. solteirx
-9. jantar
-10. role no sábado netflix no domingo
-11. sim 
-12. pelo andar da carruagem não
-13. não
-curte que eu mando</t>
+    <t>saudade quando netflix lançava uns reality show nada a ver</t>
+  </si>
+  <si>
+    <t>1 hr rolando pela netflix e to quase assistindo diário de uma paixao de novo https://t.co/vxhoyygtng</t>
+  </si>
+  <si>
+    <t>@culleniconic @mbxnoist @gincanafriend a própria netflix colocou sem acento https://t.co/pehdnu5lvc</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estrelará série espanhola de ação da netflix https://t.co/cwgxgzrlsq</t>
+  </si>
+  <si>
+    <t>sinto que já vi tuod q tinha na netflix??</t>
+  </si>
+  <si>
+    <t>um alô pros fãs de reality da netflix. 
+a tudum encomendou novas temporadas de get organized with the home edit (2ªt) e dream home makeover (3ªt) e definiu uma data de estreia no verão norte-americano para sparking joy with marie kondo. https://t.co/k1vscqld1b</t>
+  </si>
+  <si>
+    <t>@thpportilla anahí e alfonso precisam estar, faça algo @netflix</t>
+  </si>
+  <si>
+    <t>a ludovica separou produções do streaming com looks para te inspirar; veja
+via @souludovica 
+https://t.co/cr8atbveqz</t>
+  </si>
+  <si>
+    <t>@mariinalopesc @visoesdabia @lspwuvjiiob_ mano eu queria reassistir 🥺🥺🥺🥺🥺🥺 pq netflix pq??????</t>
+  </si>
+  <si>
+    <t>@vitao_guedes @vivobr a @clarobrasil não é diferente. enfiaram um pacote netflix na minha conta clandestinamente. daí vc entra em contato com eles por aqui e depois os caras desaparecem. não resolvem nada!! e seguem cobrando o serviço que não solicitei</t>
+  </si>
+  <si>
+    <t>nao acredito q a netflix vai fazer isso.... https://t.co/xchxaodnef</t>
+  </si>
+  <si>
+    <t>@netflixbrasil os livros q esperem, vou ver a série antes netflix kkkkkkkkk https://t.co/4tf0ivaapr</t>
+  </si>
+  <si>
+    <t>queria assistir friends mas nao tem mais friends na netflix wue vida triste</t>
+  </si>
+  <si>
+    <t>netflix já pode anunciar o nikolai https://t.co/93jhw0szyd</t>
+  </si>
+  <si>
+    <t>eae netflix cadê a 4ª temporada de cobra kai</t>
+  </si>
+  <si>
+    <t>@netflixbrasil @shadowandbonebr avisa que ela é melhor de todas, netflix https://t.co/vm8jih9hw5</t>
+  </si>
+  <si>
+    <t>que tristeza ver como o nível dos filmes caiu tanto. os indicados ao oscar, muitos na grade da netflix, são filmes que não merecem estar na sessão da tarde.</t>
+  </si>
+  <si>
+    <t>porque o catalogo tem títulos que ficarão incompletos? porque não informar ao cliente com antecedência @netflix ? assim não perderiamos tempo com series inacabadas!</t>
+  </si>
+  <si>
+    <t>@netflixbrasil meu deus eu tava esperando tanto por esse momento, netflix, obrigada</t>
+  </si>
+  <si>
+    <t>tô sem netflix e tô doido pra termina de assistir the ranch</t>
+  </si>
+  <si>
+    <t>mano eu assisti completamente todos os filmes de romance e dança na netflix zerei tudo . e os outros filmes de carro e coisa do tipo tbm . isso que da de nn fazer nada o dia todo</t>
+  </si>
+  <si>
+    <t>@netflixbrasil dona netflix avisa que a alina é a rainha 🛐🛐</t>
+  </si>
+  <si>
+    <t>eu já assisti metade das coisas do catálogo da netflix mas n termino suits</t>
+  </si>
+  <si>
+    <t>netflix avisa que ela é a maior de todas https://t.co/wj5pm9ygui</t>
+  </si>
+  <si>
+    <t>tiraram o melhor filme do will smith da netflix meu dia foi de ruim a bosta</t>
+  </si>
+  <si>
+    <t>tenho acesso a netflix: assisto crunchyroll o dia inteiro. 
+perco o acesso a netflix: não quero assistir nada pq tudo o que me da vontade de ver é na netflix.</t>
+  </si>
+  <si>
+    <t>alguém avisa pro netflix que em “a sentinela” não existe soldada, todo dia eu entro na esperança de corrigirem mas talvez a militância seja mais forte que o português bem escrivido e dizido</t>
   </si>
   <si>
     <t>como vcs conseguiram tirar print da tela da netflix?????????? https://t.co/n3rfd7ybph</t>
   </si>
   <si>
-    <t>@pist_the na dublagem da netflix ele fala "tasca limão nele"</t>
-  </si>
-  <si>
-    <t>queria tanto olhar fronze hj mas não tem mais na netflix 💔</t>
-  </si>
-  <si>
-    <t>é crime só ter 4 temporadas viu netflix sua puta piranha vadia @netflixbrasil</t>
+    <t>nova série da @netflixbrasil com @mariekondo deve estrear entre junho e setembro:
+https://t.co/fcbastirbb https://t.co/ckyhxdeory</t>
+  </si>
+  <si>
+    <t>alguém paga a netflix p mim</t>
+  </si>
+  <si>
+    <t>🎥hollywood | ryan murphy e ian brennan (2020)
+logo após a 2ª guerra mundial, hollywood atrai jovens atores, roteiristas e diretores dispostos a enfrentar barreiras étnicas, de gênero e sexualidade, mantidas até então pela elite cinematográfica. (netflix)</t>
+  </si>
+  <si>
+    <t>queria só 30 rock na netflix ou prime</t>
+  </si>
+  <si>
+    <t>@malu_dos_crr akame ga kill, eu já te faleeei e tem na netflix</t>
+  </si>
+  <si>
+    <t>@allebasi_izzy @zoyakanej mamma mia,eu tenho o 1 no drive se quiser o 2 tem na netflix (que dá lily como a donna)
+https://t.co/b6hobugipj</t>
+  </si>
+  <si>
+    <t>brigamos com o estagiário da netflix então 0 promo pra gente, viu!? kkkkkkkk</t>
+  </si>
+  <si>
+    <t>kkkkkkkkkkkkk netflix se recusou a divulgar o filme da lali https://t.co/strwcpzsjt</t>
+  </si>
+  <si>
+    <t>@itsprousehart_ sim, o pior eh que os gringos mete moh pau nela eh todos os br's que eu conheço amaram ela. e pra netflix eh a opinião deles que importa</t>
+  </si>
+  <si>
+    <t>se algum dia o japao parar de fazer serie pra netflix acho que minha mae entra em colapso</t>
+  </si>
+  <si>
+    <t>@_gabrizoca não odeie não tem doctor who, sabe oq é não ter na netflix? muito triste!</t>
+  </si>
+  <si>
+    <t>loucuras de amor,explicando o novo sucesso da netflix. https://t.co/uogdpcjduz via @youtube</t>
+  </si>
+  <si>
+    <t>@itsuperduper @design_saturn adm,assim pra colocar de icon no perfil da netflix, qual?
+louis fogo ou rabisco? https://t.co/a7iqv82ddl</t>
+  </si>
+  <si>
+    <t>eu to maluco 🤪😜🤪😜🤪😜🤪😜 eu to na chuva 🌧️🌧️🌧️🌧️🌧️🌧️🌧️ eu to jojozado 🤪😜🤪😜🤪🤪😜 eu to jojozado ⚽⚽⏩🇧🇷🖤⏩🇧🇷🙅‍♂️⏩🇧🇷🙅‍♂️⏩🇧🇷 é jojo  porra🖤alo 📞📞📞📞 ai irmão 🗣️🗣️🗣️ é a tropa de jojo na netflix😎😎😎😎 vamoooooo eu to maluco 😜😜🤪😜🤪🤪 https://t.co/qldv7bx76i</t>
+  </si>
+  <si>
+    <t>hj é certo ter aquele chapa quente  mais netflix 😌</t>
   </si>
   <si>
     <t>eu so quero o wylan netflix é pedir de mais pelo wylan https://t.co/sd7xpbokio</t>
   </si>
   <si>
+    <t>@omelhorluiz @netflix te marquei? https://t.co/kmzzcjmgmo</t>
+  </si>
+  <si>
+    <t>metendo one piece aproveitando que tem legendado na netflix pra tuique assistir</t>
+  </si>
+  <si>
+    <t>hj nao quero mais nada além de um namorado fazendo cafuné em mim com netflix e brigadeiro</t>
+  </si>
+  <si>
+    <t>@netflixbrasil ela é tão fofa netflix vou colocar em um potinho e guardar pra sempre  https://t.co/bzhslpbmtj</t>
+  </si>
+  <si>
+    <t>netflix cancela spin out e lança outra série de patinação que palhaçada é essa</t>
+  </si>
+  <si>
+    <t>sempre tive vontade de ficar em casa a tarde curtindo uma netflix mas néra assim q eu queria naoooo</t>
+  </si>
+  <si>
+    <t>eu nunca vou perdoar a netflix se ela não soltar a 2 temporada de luna nera de vdd</t>
+  </si>
+  <si>
+    <t>filme bom é curioso... vejam! seria um filme de aviso? já assistiu a “tribes of europa” na netflix?
+https://t.co/ggc0hhqsm6</t>
+  </si>
+  <si>
+    <t>chuvinha ok
+netflix ok
+prime video ok
+disney+ ok
+pipoca ok
+coquinha gelada ok
+só falto o dengo :/</t>
+  </si>
+  <si>
+    <t>🚨 tentativa de interação
+qual a melhor série da netflix na opinião de vcs?</t>
+  </si>
+  <si>
+    <t>@tercalivre com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>o dia todo trancada no quarto vendo netflix 😍😍🥳</t>
+  </si>
+  <si>
+    <t>não tem true beauty na netflix??????</t>
+  </si>
+  <si>
     <t>hoje a noite vou me contentar com netflix</t>
   </si>
   <si>
-    <t>me falem uns filmes mt bons pra eu ver na netflix, amazon, disney+ e derivados pfff</t>
-  </si>
-  <si>
-    <t>resolver meus problemas ou ver série ruim da netflix?</t>
-  </si>
-  <si>
-    <t>@bbb_coment @faahlso_ @tuitajulie kkkkkkk essa daí só se ficaria com outra mulher sob as câmeras da netflix, pelo pink money. igual uma cantora de funk aí que se diz bi mas so pega homen</t>
-  </si>
-  <si>
-    <t>catálogo da netflix tá um lixo minha nossa</t>
-  </si>
-  <si>
-    <t>@lalifasbr @ale_eufrasio @netflixbrasil @esposbrasil literalmente todo mundo pergunta sobre a série que gosta na netflix e pede divulgação, pergunta de data de estreia e etc. não vejo nada de mal nisso</t>
-  </si>
-  <si>
-    <t>@dibnysus não recomendo assistir na netflix pq eles traduziram a 2 imagem errado e trocaram a ending que é maravilhosa 😭</t>
-  </si>
-  <si>
-    <t>@_ciar4_ okok e ana plmdds sherlock vai sair da netflix daqui a 13 dias ent qnd tiver livre p ver chama</t>
-  </si>
-  <si>
-    <t>@hessaflame amgg eu amava, até que um dia minha conta na netflix bugou e não sei onde parei, ai não terminei</t>
-  </si>
-  <si>
-    <t>acabei de ver que a netflix criou outra série de patinação no gelo invés de ter renovado spinning out</t>
-  </si>
-  <si>
-    <t>@netflixbrasil @brunogagliasso lupin netflix, cadê?
-https://t.co/jew3jdua8q</t>
-  </si>
-  <si>
-    <t>@perobensee eu acho muito bom pq por mais que sejam "filmes interativos" eles não funcionariam bem fora do video game, não teria a mesma fluidez e imersão (basta ver bandersnatch ou qualquer coisa interativa da netflix e comparar com what remains of edith finch por exemplo)</t>
-  </si>
-  <si>
-    <t>vai ter demon slayer na netflix 
-agr eu nn tenho mais desculpa pra nao assistir 👍</t>
-  </si>
-  <si>
-    <t>não tem true beauty na netflix??????</t>
-  </si>
-  <si>
-    <t>@zzizzarv @shaygrudolph é a atriz que fez a dawn na 1° temporada da série baby sitters club da netflix e agora ela faz a america chavez na marvel (inclusive vai estar no novo filme do doutor estranho)</t>
-  </si>
-  <si>
-    <t>assistindo lagoa azul na netflix</t>
-  </si>
-  <si>
-    <t>@alicia0taria nunca vi, tem na netflix eh amg?</t>
-  </si>
-  <si>
-    <t>filme novo da netflix mt bom assistam</t>
-  </si>
-  <si>
-    <t>quais são os melhores doramas que tem na netflix?</t>
-  </si>
-  <si>
-    <t>a jeni excluiu minha conta da netflix na casa dela minha filha?? n posso fazer nada mesmo ok me demite ent caralho que ódioooo n vejo a hora de sair daqui</t>
-  </si>
-  <si>
-    <t>comédia policial à brasileira, “cabras da peste” estreia na netflix https://t.co/4hy4mnv5mk</t>
-  </si>
-  <si>
-    <t>@sonia77mesquita @cate_carrington @blushhhhhhhhh eu ainda tenho netflix... felizmente 🤣</t>
-  </si>
-  <si>
-    <t>eu não tenho netflix para assistir sky rojo. pobre não tem um dia de paz</t>
-  </si>
-  <si>
-    <t>@_chei a série está em pre-produção pelo netflix, com produção do filho do gabriel garcia marques</t>
-  </si>
-  <si>
-    <t>não estou tendo tempo de assistir nem um filme na netflix.</t>
-  </si>
-  <si>
-    <t>@isaftany estamos achando que ele vai trabalhar com o bruno gagliasso na netflix</t>
-  </si>
-  <si>
-    <t>@srchances ve logo o anime da netflix
-so 10 eps
-rapidinho se acaba
-chorandp
-se lembre disso
-se acaba chorando</t>
-  </si>
-  <si>
-    <t>#tbt para esse dia icônico que louis hofmann (jonas, de dark) falou sobre “estar de volta filmando a s2 de the rain” e lucas repostou “obrigado ao meu dublê de cenas difíceis. não conseguiria sem você” 
-uma colaboração, hein netflix! 👀 
-📸 louishofmann https://t.co/jp0apzx9lk</t>
-  </si>
-  <si>
-    <t>só queria ta deitadinha vendo um netflix f1 com as cias 😍🌈</t>
-  </si>
-  <si>
-    <t>meu deus a netflix fez uma série sobre piratas?????? tô meio em dúvida se é formato história ou documentário, e vamos ver se consegue chegar aos pés de black sails</t>
-  </si>
-  <si>
-    <t>@alderaansleia por que você está me indicando filme original netflix, geovana? o que eu fiz de errado pra você?????</t>
-  </si>
-  <si>
-    <t>meu a baghra sei lá o nome como escreve batendo na alina com a bengala oi eu que pedi ta netflix</t>
-  </si>
-  <si>
-    <t>jojo vai lançar na netflix meu cérebro de jojofag está simplesmente explodindo com serotonina finalmente um motivo pra viver eu vo rever tudo</t>
-  </si>
-  <si>
-    <t>#netflix testa função para impedir compartilhamento de senhas. vem ver: https://t.co/b7anmmkoid https://t.co/i9rcoliaqz</t>
-  </si>
-  <si>
-    <t>na minha opinião, todo mundo deveria assistir isso...
-https://t.co/fh3hjupypv</t>
-  </si>
-  <si>
-    <t>@bhtgds já viu sem maturidade pra isso? animação boa
-original netflix</t>
-  </si>
-  <si>
-    <t>chuvinha boa pra tá com a @ assistindo netflix</t>
-  </si>
-  <si>
-    <t>meu, tem uma serie documentário na netflix que fala de medicina n convencional né, ai tem oleo essencial, homeopatia essas coisas e tem relatos que deram certo e relatos que deram errado</t>
-  </si>
-  <si>
-    <t>@_animese jojo na netflix talvez dublado 
-kimetsu na netflix dublado 
-tp 2 de kimetsu  
-filme de kimetsu
-2 eventos grabdes de jojo onde provavelmente vao anunciar a parte 6
-klr minha sorte virou do nada</t>
-  </si>
-  <si>
-    <t>essa aí dava uma boa série pra netflix</t>
-  </si>
-  <si>
-    <t>eu tô triste de verdade com a retirada de merlí da netflix. não entra na minha cabeça como podem tirar uma série tão foda, necessária e rica em conhecimento que eles mesmos produziram 😭</t>
-  </si>
-  <si>
-    <t>@_otakusbr netflix indo de mal a pior a cada dia. slk</t>
-  </si>
-  <si>
-    <t>o mesmo ator q fez um personagem de 30 anos em locke key interpretando um adolescente em ginny &amp;amp; georgia
-se isso n diz algo sobre as decisoes de cast da netflix kkkk</t>
-  </si>
-  <si>
-    <t>hj o dia tá propício pra assistir muitos filmes na netflix. :) ... já comecei com um "dia do sim". agora vamos de filme repetido kkkkk acho que vou começar com "dançarina imperfeita" 😍😍🤩🤩</t>
-  </si>
-  <si>
-    <t>#cinema | indicado ao oscar, curta palestino entra no cardápio da netflix - https://t.co/tdbiwyvsgy https://t.co/ckdnakaqxs</t>
-  </si>
-  <si>
-    <t>atinys vão no link nesse tweet e coloquem como sugestão:
-"imitation 이미테이션 by kbs2" 
-em seguida envie, vc n precisa ter uma conta pra  poder fazer a sugestão, vamos por imitation na netflix! @ateezofficial https://t.co/jk66klvolo</t>
-  </si>
-  <si>
-    <t>jura netflix?? achei que era ano quem vem, já que vocês não falam nada https://t.co/bi5rsdygne</t>
-  </si>
-  <si>
-    <t>se a netflix não mostrar o gp da turquia eu serei obrigada a cometer um crime</t>
-  </si>
-  <si>
-    <t>nao acredito que a netflix cancelou spin out pra fazer essa outra serie de patinação no gelo meia boca https://t.co/whny55rcxb</t>
-  </si>
-  <si>
-    <t>bring the light! confira o novo vídeo promocional de ‘shadow and bone’, que estreia dia 23 de abril na netflix. ansiosos? #shadowandbone 
- https://t.co/gxgltz5dnb</t>
-  </si>
-  <si>
-    <t>eu nunca vou perdoar a netflix se ela não soltar a 2 temporada de luna nera de vdd</t>
-  </si>
-  <si>
-    <t>bruno gagliasso tem estreia confirmada na netflix e anúncio brinca com polêmica em noronha https://t.co/urbhktcym5</t>
-  </si>
-  <si>
-    <t>poxa netflix, lança mais uma temporada de castlevania ai pra eu ter um pouquinho de felicidade pf</t>
-  </si>
-  <si>
-    <t>meu deis essa série de shadow and bone vai ser fantástica netflix lança logo eu não aguento esperar mais naoooo</t>
-  </si>
-  <si>
-    <t>tiraram o melhor filme do will smith da netflix meu dia foi de ruim a bosta</t>
-  </si>
-  <si>
-    <t>como se a manu fosse um mega influencer né? manu tá ganhando horrores com os contratos da netflix malmente ela posta um stroys kkkkkkkk https://t.co/s6enhpwhkf</t>
-  </si>
-  <si>
-    <t>the expanse era tao bom e tbm saiu da netflix, ai caralho mesmo</t>
-  </si>
-  <si>
-    <t>meu professor de direito internacional pegou pesadíssimo em mandar fazermos uma resenha crítica comparando o caso do chile que foi condenado por censurar um filme que envolvia a fé cristã vs. o caso do especial de natal do porta dos fundos que foi retirado da netflix...</t>
-  </si>
-  <si>
-    <t>ta tao perfeito netflix pelo amor de deus n estrague https://t.co/4zpjwsht2p</t>
-  </si>
-  <si>
-    <t>a netflix deve achar que meu perfil é de criança pq só me recomenda desenho e filmes de família</t>
-  </si>
-  <si>
-    <t>mano, como assim como treinar seu dragão vai sair da netflix</t>
-  </si>
-  <si>
-    <t>sozinho d cs, fumando um kank vendo netflix 😅🍁</t>
-  </si>
-  <si>
-    <t>lembrei de quando achei um diário no meio de uns livros usados. as passagens icônicas. as brigas com o namorado. os dramas familiares. os perrengues com dinheiro. todo o arco do início da vida adulta retratados. melhor que muita série da netflix.</t>
-  </si>
-  <si>
-    <t>jojo vai chegar na netflix mês q vem, será q eu finalmente vou começar a assistir e virar jojofag?</t>
-  </si>
-  <si>
-    <t>alguém me empresta uma netflix ai assistir um romance kkkkk</t>
-  </si>
-  <si>
-    <t>netflix eu te odeio, eu só queria assistir meu friends de novo</t>
-  </si>
-  <si>
-    <t>@seenyoucry então, demora uns episódios pra gostar pq eles dão uma enrolada, mas achei um anime bom até kakaka
-tem a primeira temporada na netflix e os episódios são bem curtinhos</t>
-  </si>
-  <si>
-    <t>quero trocar a foto da netflix mas a jennie é tão linda q fico com dó de tirar 😭</t>
-  </si>
-  <si>
-    <t>não perdoo a netflix queria muito saber como iria ficar sterling e april e como a família ia ficar com os 838338 segredos</t>
-  </si>
-  <si>
-    <t>eu assisti o show não faz.sentido na netflix e  achei horrível  kkkkkk mas não me dei por convencida,um dos maiores youtubers do brasil,não podia ser só  aquilo...
-resultado: me apaixonei pelo canal e meu davi tbm... https://t.co/chqnznizms</t>
-  </si>
-  <si>
-    <t>se eu assisto série é p espairecer se fosse p passar raiva eu assistia as entrevistas com o presidente portanto netflix colabore que saco</t>
-  </si>
-  <si>
-    <t>queria mais séries norueguesas na netflix, amo aquele país, é tão lindo 😢</t>
-  </si>
-  <si>
-    <t>acabei de assistir o filme "por trás da inocência" da netflix. me interessou por ninguém estar entendendo o filme, e eu entendi ele perfeitamente. será que sou doida? 😂</t>
-  </si>
-  <si>
-    <t>gosto da ideia de assistir bbb como se fosse um reality netflix q já tem tudo gravado e eu não tenho como intervir em nada</t>
-  </si>
-  <si>
-    <t>@eduardoleite_ @corsan_oficial até a chuva https://t.co/sl8hjsyktt</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. não 🙃
-2. uma
-3. capricórnio
-4. espero que sim
-5. apegado
-6. não
-7. nenhum
-8. solteiro
-9. jantar fora
-10. netflix em casa
-11. sim
-12. espero 🙏
-13. 
-curte que eu mando</t>
-  </si>
-  <si>
-    <t>graças ao netflix eu virei um apaixonado por f1. @netflixbrasil @f1</t>
-  </si>
-  <si>
-    <t>@brownskiingrl aproveita que tem ambos na netflix, e fmab é curto https://t.co/kklc8ey8kf</t>
-  </si>
-  <si>
-    <t>essa fanfic vai ser basicamente uma cópia desse filme, vou mostrar quem vão ser os personagens. 
-lembre-se assista o filme!! olhos de gato na netflix</t>
-  </si>
-  <si>
-    <t>@beccapires vocês estão assistindo muitas série latinas no netflix</t>
-  </si>
-  <si>
-    <t>comendo rei do pastelzinho, netflix e chororo</t>
-  </si>
-  <si>
-    <t>@imirnac eu ai quando tinha netflix</t>
-  </si>
-  <si>
-    <t>meu deus o meu irmão falou que vai passar kimetsu no yaiba na netflix eu vi o anime inteiro e to mo feliz mesmo ja tendo visto o anime aaaaaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>@pevensievans acorda best,daqui a pouco a netflix lança a braba</t>
-  </si>
-  <si>
-    <t>@_animese porra de jojo na netflix. eu quero a adaptação da parte 6 aaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>@netflixbrasil netflix e a segunda temporada de unité 42? 😭😭</t>
-  </si>
-  <si>
-    <t>a netflix liberou mais um vídeo de shadow and bone da alina treinando ahhhhhhhhh que dia</t>
-  </si>
-  <si>
-    <t>@missbushiido @op_netflix_fan @angelicaefrem quero o hiluluk assim no live action, com cara de doido mesmo</t>
-  </si>
-  <si>
-    <t>realmente essa série nova de piratas da netflix é um documentário encenado com baixo orçamento, mas não é ruim</t>
-  </si>
-  <si>
-    <t>o nome é six of crows e vcs colocam 3 na capa netflix pisou na bola nessa ai https://t.co/xopdacnhxp</t>
-  </si>
-  <si>
-    <t>seu futuro na netflix? se isso é um sonho, eu não quero acordar 😭😍 https://t.co/uwxlvhkq2q</t>
-  </si>
-  <si>
-    <t>alguém me indica uma série ou um filme massinha da netflix</t>
-  </si>
-  <si>
-    <t>@soulmoontae amg eu também!!! não vejo a hora de sair na netflix pra maratonar. saudades demais do siwan com cara de neném 🥺</t>
-  </si>
-  <si>
-    <t>isto é das coisas mais burras que já ouvi. estávamos melhor a caçar todos os dias para comer e a morrer aos 30 com uma doença random qq, ou a ver netflix no sofá enquanto esperamos pelo uber eats? https://t.co/qiqy22cmgi</t>
-  </si>
-  <si>
-    <t>me indiquem filmes clichês na netflix</t>
-  </si>
-  <si>
-    <t>@_rodrigomattos_ qual a relação do futebol com a pandemia? os estádios estão com público? algum jogador esta infectado jogando? vai aglomerar em casa? então fecha o big bista e netflix, mandou o pvc</t>
-  </si>
-  <si>
-    <t>@davidwe32380311 @fabiorrluz74 @portugassis verdade pois fate tem um público mais nicho, kimetsu vai vir dublado em pt br em abril na netflix aí talvez mais pessoas conheçam e o manda vende pra caraí.</t>
-  </si>
-  <si>
-    <t>esse filme poderia ser facilmente protagonizado por bella thorne.
-"por trás da inocência" na netflix.
-https://t.co/qrlstauvsl</t>
-  </si>
-  <si>
-    <t>🎬07- chilling adventures of sabrina | 2020
-• diretor: roberto aguirre-sacasa
-• gênero: terror
-• netflix
-⭐️⭐️⭐️ https://t.co/abfhwycgxl</t>
-  </si>
-  <si>
-    <t>velozes e furiosos vai sair do catalogo da netflix, declaro aqui a minha tristeza e indignação</t>
-  </si>
-  <si>
-    <t>@lgriao @revargasbr @netflix e também contrata uns lacradores de fernando de noronha , tô fora</t>
-  </si>
-  <si>
-    <t>@fvzstyles filme delas que tem na netflix</t>
-  </si>
-  <si>
-    <t>ansiosa desde já https://t.co/s8atkposqf</t>
-  </si>
-  <si>
-    <t>alguém me passa a conta da netflix só por esse fim de semana pfv quero ver dts3</t>
-  </si>
-  <si>
-    <t>sim conseguiu ser melhor com jojo na netflix aaaaa</t>
-  </si>
-  <si>
-    <t>minha saudade tem nome, sobrenome, elenco, ótima atuação e um casal com química. a verdade é que spin out tinha tudo para ser um sucesso com várias temporadas. é uma pena que a netflix não tenha entendido essa obra de arte. https://t.co/copx6odnsx</t>
-  </si>
-  <si>
-    <t>desisti de ver o documentário do chico buarque e decidi ver dawson's creek na netflix</t>
-  </si>
-  <si>
-    <t>@figurante34 @op_netflix_fan @missbushiido pq vc fez isso comigo eu agora tô chorando no meio do expediente 🤧🤧🤧</t>
-  </si>
-  <si>
-    <t>fazer delineado p ficar em casa de pijama assistindo netflix</t>
-  </si>
-  <si>
-    <t>ia ve um filme mas digitei neopets ao inves de netflix e so me toquei 20 min dps navegando no site sem rumo</t>
-  </si>
-  <si>
-    <t>@gabiu_twt eu tenho certeza que ela teria tido um revival na carreira numa série da netflix</t>
-  </si>
-  <si>
-    <t>@rodrigo_pazm viu onde paz? netflix? tô vendo o documentário sobre as guerras dos samurais, muito legal também</t>
-  </si>
-  <si>
-    <t>a netflix na hora de montar um personagem latino https://t.co/yozdtlh06r</t>
-  </si>
-  <si>
-    <t>que diferença faz quarentena se vc não trabalha não estuda só fica na netflix  e em casa fumando maconha e  não faz um nada o filha da puta</t>
-  </si>
-  <si>
-    <t>o dia mais temido da minha vida chegou, a pessoa que eu ratiava netflix mudou de senha</t>
-  </si>
-  <si>
-    <t>brigamos com o estagiário da netflix então 0 promo pra gente, viu!? kkkkkkkk</t>
-  </si>
-  <si>
-    <t>e eu descobri so agora que o titus de unbreakanle kimmy shmidt  apresenta esse vem cantar na netflix como eu amo este gay meodeus</t>
-  </si>
-  <si>
-    <t>ligar tv agora só pra assistir netflix, tô ficando com mais pânico com as notícias do covid! 😢😓😓</t>
-  </si>
-  <si>
-    <t>@fraannnnnnnnn final de temporada nas séries da netflix</t>
-  </si>
-  <si>
-    <t>bora netflix lança uma série boa aí pra mim poder me alienar com algo bom</t>
+    <t>@rodrigojames a parada que me espanta é como eles não sabem vender o próprio serviço. eles tentam competir com o netflix quando deviam se posicionar como uma versão mais crescida do disney+.</t>
+  </si>
+  <si>
+    <t>como assim sherlock sai do catálogo da netflix dia 30</t>
+  </si>
+  <si>
+    <t>impressionante mano, é só eu ver o anime em site pirata que ele vai pra netflix, tiração https://t.co/nrztmyhauq</t>
+  </si>
+  <si>
+    <t>@nebels @renatobarrosbr @knalquestionese com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
   </si>
   <si>
     <t>indicado ao oscar, curta palestino entra no cardápio da netflix; leia mais no blog orientalíssimo, por @diogobercito 
 https://t.co/jee0mwjgb2</t>
   </si>
   <si>
-    <t>1. não
-2. 1
-3. peixes
-4. não
-5. apegada
-6. nunca
-7. provavelmente ja fui
+    <t>sobre relacionamentos 
+1. não 
+2. 2
+3. sla kkkk
+4. não 
+5. depende 
+6. sla
+7. n sei
 8. solteira
-9. mandar flores  
-10. netflix em casa 
-11.  sim
-12. nn
-13. nn</t>
-  </si>
-  <si>
-    <t>na madrugada de hoje pra amanhã tem nada mais nada menos que;
-falcão e soldado invernal
-f1 drive to survive 3
-obrigado disney e netflix 🥶</t>
-  </si>
-  <si>
-    <t>meu rolê todos os dias youtube&amp;gt;&amp;gt;netflix&amp;gt;&amp;gt;google meet</t>
-  </si>
-  <si>
-    <t>mlk vai te jojo na netflix
-dessa vez eu assisto tudo
-https://t.co/3bl4ndwbf1</t>
-  </si>
-  <si>
-    <t>@gustavin1x me chama no wpp que te passo outras da netflix</t>
-  </si>
-  <si>
-    <t>tava lá na netflix naquela aba de lançamento daí achei lá gostei da sinopse e assisti 
-we love you kyndra https://t.co/2s2nmoknjy</t>
-  </si>
-  <si>
-    <t>jamie foxx vive quatro personagens em nova série da netflix; veja trailer &amp;gt; https://t.co/zaeirxohim https://t.co/v9tewfofsp</t>
-  </si>
-  <si>
-    <t>acabei de ver o show do @maumeirelles na netflix. parabéns amigo ta horrível!!!!</t>
-  </si>
-  <si>
-    <t>viciada em documentário sobre tecnologia 
-o código bill gates (netflix) é 10/10 e print the legend (netflix) também</t>
-  </si>
-  <si>
-    <t>esse filme silenciadas da netflix 
-pica demais né amei</t>
-  </si>
-  <si>
-    <t>o anime twt eh muito engraçado tinha uma mutual reclamando que jojo entrou na netflix e outra comemorando na mesma hora https://t.co/dub6wu44eu</t>
-  </si>
-  <si>
-    <t>eu: “you” é a pior série da netflix, sem condições
-eu tbm: vou ver só mais um episódio</t>
-  </si>
-  <si>
-    <t>hj era só eu ela uma netflix e um brigadeiro 😭</t>
-  </si>
-  <si>
-    <t>queria indicações de filmes na netflix?🤔🙄</t>
-  </si>
-  <si>
-    <t>@fabriciocarlet1 acho que a força da marca disney pesa muito. mas o produto em si é fraco. 
-catálogo muito reduzido. assinei 2 meses e cancelei. nem a minha filha tava gostando, salvo um ou outro filme. netflix e prime vídeo eu mantenho.</t>
-  </si>
-  <si>
-    <t>eae netflix cadê a 4ª temporada de cobra kai</t>
-  </si>
-  <si>
-    <t>@nsuspenso se a netflix lançar certo 
-do jeito que a netflix é vai lançar todo incompleto 
-só a parte 1 e 3 kkkkkkkkkkkkkkjkjk
-igual bob esponja kkkkkkkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>só queria ta de boa vendo um netflix cm a gata mas falto a gata...</t>
-  </si>
-  <si>
-    <t>feliz pra krl que o tigre branco da netflix foi indicado ao oscar tomara que ganhe</t>
-  </si>
-  <si>
-    <t>eu só quero um pouquinho de serotonina e a única pessoa que pode me dar isso é a @netflix com a segunda temp de julie and the phantoms</t>
-  </si>
-  <si>
-    <t>eu estava vendo aquele interativo do daniel radcliffe na netflix, e passei meia hora rindo e me perguntando "que porra é essa que eu estou vendo?"</t>
-  </si>
-  <si>
-    <t>@mariinalopesc @visoesdabia @lspwuvjiiob_ mano eu queria reassistir 🥺🥺🥺🥺🥺🥺 pq netflix pq??????</t>
-  </si>
-  <si>
-    <t>apenas os conteúdos exclusivos, como programas, séries e filmes exigem uma assinatura paga. 
-eu acho essa estratégia muito inteligente, e em terras de globoplay e netflix, seria uma boa!</t>
-  </si>
-  <si>
-    <t>@majullpz netflix deu na telha de fazer serie de magia agr do nada</t>
-  </si>
-  <si>
-    <t>se a suzy e o joohyuk não ficarem juntos eu vou esmurrar a netflix.</t>
-  </si>
-  <si>
-    <t>foi a primeira coisa que apareceu quando eu abri a netflix 
-we love you kyndra https://t.co/h2pyxjqvjy</t>
-  </si>
-  <si>
-    <t>@cshimada hahaha brigado lindissimaa❤️ olha se depender das materias q eu to tendo tem um processo longo até a netflix hahahah mas fé</t>
-  </si>
-  <si>
-    <t>lee junyoung num filme da netflix ¿¿¿¿¿¿¿¿
-meu deus fui eu que pedi sim
-tomara que finalmente ele seja reconhecido 😭 https://t.co/oz8tcxweik</t>
-  </si>
-  <si>
-    <t>pro pessoal que polariza as eleições 2022 entre lula e bolsonaro, indico ver (ou rever):
-o mecanismo (netflix) 
-a lei é para todos 
-retrato narrado (spotify) 
-pra refrescar a memória e ver que nenhum deles merece chegar ao segundo turno, caso se candidatem.</t>
-  </si>
-  <si>
-    <t>netflix + chuva só falta um love 😴</t>
-  </si>
-  <si>
-    <t>white tiger, filme indicado ao oscar e tá  netflix, me fez ter um choque de realidade com a índia.
-eu achei que atualmente as coisas eram bem melhores lá, mas as coisas são piores lá do que aqui, por incrível que pareça.</t>
-  </si>
-  <si>
-    <t>@notescrupulos e se tu ass tem a obrigação de ass dps a entrevista da oprah, tem na netflix também!! vale a pena demais, eu recomendo pra todo mundooo</t>
-  </si>
-  <si>
-    <t>vai se foder netflix vai tomar no meio do seu cu eu te odeio por fingir que helnik e o wylan nao existem eu te odeio eu preferiria mil vzs uma capa so com o kaz entao enfia no seu rabo esta merda https://t.co/kezpe1nqzv</t>
-  </si>
-  <si>
-    <t>pra esse dia friozinho, café, netflix e moletom 🤍</t>
-  </si>
-  <si>
-    <t>pra quem não me conhece eu sou a netflix de aruanda kkkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>a jessie mei li de alina netflix você entregou tudo</t>
-  </si>
-  <si>
-    <t>@aplantonista @_marciovinicius estás vendo hp por onde? eu comecei a ver, vi até o quarto, mas saiu da netflix 😭</t>
-  </si>
-  <si>
-    <t>@canaldocoelho_ @meuxbox os caras são mal intencionados e capciosos, utilizam de qualquer coisa não muito clara contra o xbox. mas convenhamos, esse marketing tabajara da microsoft é coordenado por quem? seu creysson? antes tava ruim, trouxeram o cara da netflix e parece que ficou pior... 🤓 https://t.co/lsegb18vtx</t>
-  </si>
-  <si>
-    <t>@euoseuamor @elleenzinha__ compartilha a netflix aí mô 😞</t>
-  </si>
-  <si>
-    <t>alô netflix favor colocar a última temporada de the 100 no catálogo, todo mundo já assistiu menos eu kkk</t>
-  </si>
-  <si>
-    <t>agora que tenho o amazon prime, nunca mais assisti netflix kkk é muito melhor</t>
-  </si>
-  <si>
-    <t>@fcrellan @chrismerigold @hel0vee @_pmneto mt caro pro orçamento de 2 tustao e um chiclete da netflix</t>
-  </si>
-  <si>
-    <t>essa série pit stop da netflix é muito boa. depois faço uma propaganda mais adequada aqui.</t>
-  </si>
-  <si>
-    <t>não acredito que a netflix tirou lion do catálogo não</t>
-  </si>
-  <si>
-    <t>@marvelbr @disneyplusbr @rafaela_p03 amor vou cancelar netflix pra assinar disney plus fds 😎👍</t>
+9. sla
+10. netflix 
+11. sim
+12. só deus sabe
+13. sla kkk
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>@netflixbrasil essa série vai servir tanto, avisa netflix</t>
+  </si>
+  <si>
+    <t>@drmwrx @dreamworks @netflix olae'</t>
+  </si>
+  <si>
+    <t>porra netflix coloca friends de volta no catálogo</t>
+  </si>
+  <si>
+    <t>amigaria cmg de acordo com o meu histórico da netflix ❓ https://t.co/tho6fwkgdw</t>
+  </si>
+  <si>
+    <t>até que enfim... é legal que a netflix, hbo ou outros canais façam seus documentários, mas é importante que a britney conte a sua própria versão https://t.co/zdlanbyu79</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix e sex education em? por deus não sai nunca a terceira temporada   https://t.co/nmxwinfepj</t>
+  </si>
+  <si>
+    <t>vamos todos juntos continuar lutando pela volta da nossa linda série, desistir jamais #shadowhunters #saveshadowhunters @constantinfilm @netflix @shadowhunterstv @thecw https://t.co/y6jzmtqejx</t>
+  </si>
+  <si>
+    <t>claro q a primeira coisa q ia aparecer no netflix seria fate kkkk https://t.co/t7vqfkxl0x</t>
+  </si>
+  <si>
+    <t>porra minha tl tá lotada com pedro pedindo a porra do dragon ball pra netflix q ódio viu</t>
+  </si>
+  <si>
+    <t>ok agora que jojo vai tá netflix talvez eu realmente considere assistir kkkkkk https://t.co/liuuktw661</t>
+  </si>
+  <si>
+    <t>@1zedge1 não não, me manda depois ! aqui, assiste the last dance, tem na netflix. você vai adorar, e vai ver como basquete atual é chacota comparado aquela época kkkk</t>
+  </si>
+  <si>
+    <t>preciso ter você @kat_mcnamara sempre junto do meu coração #shadowhunters #saveshadowhunters #claryfairchild @constantinfilm @netflix @thecw https://t.co/cjemf2bqao</t>
+  </si>
+  <si>
+    <t>alguem me empresta uma netflix pfvvv</t>
+  </si>
+  <si>
+    <t>bruno gagliasso tem estreia confirmada na netflix e anúncio brinca com polêmica em noronha https://t.co/urbhktcym5</t>
+  </si>
+  <si>
+    <t>netflix faça isso acontecer mlk pls https://t.co/b8mls3t5hg</t>
+  </si>
+  <si>
+    <t>@ness4richards amg tem alguns “”spin offs”” de equestria girls, e algumas temporadas de my little pony, antes tinhas os filmes, mas a netflix tirou</t>
+  </si>
+  <si>
+    <t>queria termina de ver mais a netflix tiro https://t.co/sip0a8ambs</t>
+  </si>
+  <si>
+    <t>isto é das coisas mais burras que já ouvi. estávamos melhor a caçar todos os dias para comer e a morrer aos 30 com uma doença random qq, ou a ver netflix no sofá enquanto esperamos pelo uber eats? https://t.co/qiqy22cmgi</t>
   </si>
   <si>
     <t>@emotacokkkk @op_netflix_fan @cassiomanso se o live action não for perto disso nem vejo</t>
-  </si>
-  <si>
-    <t>pouco a pouco...
-https://t.co/dmkah7l3rr</t>
-  </si>
-  <si>
-    <t>mano eu estava procurando alguma coisa para assisitir na netflix, mas não tem nada que eu goste. acho que vou assistir stranger things de novo.😚</t>
-  </si>
-  <si>
-    <t>já assisti tantas séries/filmes da netflix, que eu já não sei mais oque assistir</t>
-  </si>
-  <si>
-    <t>pelo menos hj vai ter any gabrielly convida com o booboo pra termos conteúdo pra falar nesse fandom pq se depender da netflix misericórdia</t>
-  </si>
-  <si>
-    <t>@fbe333 furo de roteiro da prr,odiei cancela a série netflix</t>
   </si>
   <si>
     <t>[📌] atiny, nós podemos pedir por #imitation na netflix, é só seguir os passos a seguir:
@@ -702,168 +497,161 @@
 4) repita o processo. https://t.co/pnmkuwgpgg</t>
   </si>
   <si>
-    <t>segundo filme hj q eu vejo na netflix e nenhum dos dois tem um final decente naam</t>
-  </si>
-  <si>
-    <t>netflix contrate agora, o maluco manja dos roteiros https://t.co/lultigcvy3</t>
-  </si>
-  <si>
-    <t>@egirldecorsa enquanto isso têm tantos talentos em busca de atuar e a netflix só escolhe os piores</t>
-  </si>
-  <si>
-    <t>saudade quando netflix lançava uns reality show nada a ver</t>
-  </si>
-  <si>
-    <t>netflix, academia, desenhar, sair com os amigos... basicamente nada mais me deixa alegre... https://t.co/3v8y0jqfmu</t>
-  </si>
-  <si>
-    <t>com certeza um dos melhores filmes que tem na netflix https://t.co/rez1tlpcvn</t>
-  </si>
-  <si>
-    <t>@mipaltan bolte 
-subscribe - https://t.co/g3clogz44p
-#dark #netflix #darkseason1 #darknetfix 
-#mumbaiindians https://t.co/txifaphg0w</t>
-  </si>
-  <si>
-    <t>netflix ta na tua mão mudar aquele final amém https://t.co/fvpjkbks3b</t>
-  </si>
-  <si>
-    <t>meu deus eu vi agora que tem voltron na netflix https://t.co/nmlp37b2cx</t>
-  </si>
-  <si>
-    <t>chuvinha boa pra deita na cama e liga a netflix</t>
-  </si>
-  <si>
-    <t>🚨 "cabras da peste" é a nossa dica para você assistir na netflix nesta quinta-feira, conheça: https://t.co/hputu0xow0 https://t.co/sopfuewp2r</t>
-  </si>
-  <si>
-    <t>nova serie da marie kondo na netflix finalmente mal posso esperar pra sair por aí organizando tudo</t>
-  </si>
-  <si>
-    <t>serviço bom é o meu, não faz nada o dia inteiro com direito a netflix</t>
-  </si>
-  <si>
-    <t>‼️ fotos de locação oficial onde rebelde netflix está sendo gravado. supostamente seria a nova elite way school. ‼️
-mas também pode ser uma expansão da escola, como um clube de campo. o que acharam? https://t.co/cv6ae8kc0d</t>
-  </si>
-  <si>
-    <t>@walkanitta @netflixbrasil @brunogagliasso pois foi o que eu fiz, não aguentei esperar chegar na netflix kkkkkk</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. não 
-2. 1
-3. touro 😔
-4. não 
-5. apegadx
-6. depende, se for com o meu não kkk
-7. foi traidx 
-8. solteirx 
-9. jantar fora?
-10. netflix em casa? 
-11. sim
-12. não 
-13. nsei 
-curte que eu mando</t>
-  </si>
-  <si>
-    <t>mas veja só, em abril teremos não só a 1º temporada dublada de kimetsu no yaba no netflix como também teremos o lançamento do longa-metragem por aqui. :)
-a questão é: em qual plataforma ele estará disponível? https://t.co/6iw49mbgy3</t>
-  </si>
-  <si>
-    <t>só queria uns carinhos um açaí e uma netflix pra hoje</t>
-  </si>
-  <si>
-    <t>vou assistir silenciadas da netflix agora</t>
-  </si>
-  <si>
-    <t>ahahahaa
-pensa num filme kkkkkk
-#cabrasdapeste 
-#filme 
-#netflix https://t.co/nfiqjrpt8k</t>
-  </si>
-  <si>
-    <t>link errado, é um site de vendas
-mas tem pessoas real que vivem uma vida leve, com o proposito de cuidar da vida marinha em praias desertas, querendo uma vida simples, mas com um iphone bom pra ver netflix, pq a gnt gosta de minimalismo, mas tbm de rapidez
-apple te amo ainda</t>
-  </si>
-  <si>
-    <t>@cowidflys2 netflix. chama “por trás de seus olhos”</t>
-  </si>
-  <si>
-    <t>@gicarmignani to não! https://t.co/yzh01ognwe</t>
-  </si>
-  <si>
-    <t>estou conversando com uma hacker famosa num programa de mensagens anonimas me sinto numa série da netflix</t>
-  </si>
-  <si>
-    <t>pedi os dados da netflix pra minha amg e vou assistir kakeguriu</t>
-  </si>
-  <si>
-    <t>queria um anime pequeno, de 12 ou 20 eps pra assistir. precisa ter em streaming não, qualquer coisa eu baixo (mas se tiver na netflix, prime ou crunchyroll ja me adianta kkkk)</t>
-  </si>
-  <si>
-    <t>@parker_bop amg tem um site q tem todos os filmes da netflix de graça</t>
-  </si>
-  <si>
-    <t>e eu reclamando do selo da netflix na edição br. desculpa https://t.co/wkqekcjl9d</t>
-  </si>
-  <si>
-    <t>@ale_eufrasio @lalifasbr @netflixbrasil @esposbrasil estamos perguntando sobre a divulgação de uma série da plataforma, não estamos falando mal de nenhuma outra e todos fazem o mesmo. enfim, assista sky rojo na netflix e uma excelente tarde</t>
-  </si>
-  <si>
-    <t>@netflixbrasil netflix adiciona “to my star” no catálogo, é um filme coreano bl do estilo de “wish you”</t>
-  </si>
-  <si>
-    <t>kayky falou q meu quarto tá q nem hotel, c televisão c netflix , ar ventidor, cama, som kkk</t>
-  </si>
-  <si>
-    <t>“professor polvo” é um dos melhores documentários que já vi! se não ganhar o oscar eu vou ficar muito triste.
-vejam! é da netflix! lindo demais!</t>
-  </si>
-  <si>
-    <t>@netflix absolutamente ninguem pediu aquela jacket de six of crows mude aquele troço horrivel agora</t>
-  </si>
-  <si>
-    <t>eu já assisti metade das coisas do catálogo da netflix mas n termino suits</t>
-  </si>
-  <si>
-    <t>@seraineneto @_marciovinicius eu já tenho eles baixados no meu computador kkkkkk a saída de hp foi uma grande perda pra netflix e pros fãs 💔</t>
-  </si>
-  <si>
-    <t>andrea cantando bruno mars e acompanhando a letra sem ter ensaiado antes, tudo pra mim ❤️ https://t.co/ioiypzxtoq</t>
-  </si>
-  <si>
-    <t>esse lindo e amado anjo @domsherwood1 é dono absoluto do meu coração #shadowhunters #saveshadowhunters #jaceherondale @constantinfilm @netflix @thecw https://t.co/zqwamaobvd</t>
-  </si>
-  <si>
-    <t>netflix tá perdendo essa guria como roteirista</t>
-  </si>
-  <si>
-    <t>precisando de um filme top da netflix</t>
-  </si>
-  <si>
-    <t>series de adolescente na netflix são assim https://t.co/sdpegldvvx</t>
-  </si>
-  <si>
-    <t>as 6 melhores séries da netflix  sem dúvidas 😍😍
--o atirador 
--vikings
--riverdale
--vis a vis 
--lucifer 
--la casa de papel</t>
-  </si>
-  <si>
-    <t>te falar que o clima nessa semana tá tão merda, que tô considerando real pagar pra assistir o snydercut no fds. 4h de filme + 10h de drive to survive na netflix + 1h de falcão &amp;amp; soldado invernal + algumas horas de doom..acho que é alienação o suficiente pra esquecer o apocalipse</t>
-  </si>
-  <si>
-    <t>caio criou uma conta infantil pra mim na netflix kkkkkkk</t>
-  </si>
-  <si>
-    <t>seja hamilton, max, seb, ricciardo, wtv... é horrível a netflix não mostrar o momento em que um piloto se torna campeão do mundo. alias, não fazer 1 episódio dedicado a esse tema é absurdo. neste caso particular, ainda pior com um piloto q igualou um record histórico de 7 titulos https://t.co/yz3jreiui1</t>
+    <t>@fvzstyles filme delas que tem na netflix</t>
+  </si>
+  <si>
+    <t>@the_bat_22 @_animese pois é, e também vai ser uma tacada boa da netflix colocar até a parte 4,pq,além de existir o ova do rohan,o mangá aqui no brasil vai chegar na parte 4 um mês depois de ela chegar na netflix,então vai ser bom pra netflix e pra panini,também vai ser 4 dias depois do evento de jojo</t>
+  </si>
+  <si>
+    <t>que doideira tô até assustada, tava aqui procurando onde tinha sucker punch pq queria rever e esse filme n passa em canto algum aí dps de procurar no netflix, amazon prime e now, quando eu já tinha desistido...coloco na warner e o que tá dando? sucker punch amigos</t>
+  </si>
+  <si>
+    <t>tô vendo um filme da beyoncé na netflix, eu sei que ela só fez pq viu que as apimentadas tava em alta, inveja da solange?</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estreia 'santo', produção internacional da netflix.
+https://t.co/dn3bx42zbp https://t.co/au4krldy2c</t>
+  </si>
+  <si>
+    <t>@majullpz netflix deu na telha de fazer serie de magia agr do nada</t>
+  </si>
+  <si>
+    <t>netflix + chuva só falta um love 😴</t>
+  </si>
+  <si>
+    <t>@raydramas mdsss eu vi a foto sem ler a legenda e ja tava correndo pra abri a netflix aq kkkkkkkk</t>
+  </si>
+  <si>
+    <t>@annacseidel simmmm, netflix tirou a melhor (até cara gente branca)</t>
+  </si>
+  <si>
+    <t>já que a netflix não se mexe a gente faz o trabalho por eles sky rojo tomorrow</t>
+  </si>
+  <si>
+    <t>eu so queria netflix to mal alguem paga pra mim</t>
+  </si>
+  <si>
+    <t>todo dia que eu lembro que isa tkm saiu da netflix  tenho vontade de cortar os pulso</t>
+  </si>
+  <si>
+    <t>minha vida se resume a trabalhar fumar beber e assistir netflix https://t.co/0uaefqm81d</t>
+  </si>
+  <si>
+    <t>@sacifla caçadores de demônios ( netflix</t>
+  </si>
+  <si>
+    <t>meu computador tá assim tendo que trabalhar 24 horas por dia com mil janelas e programas abertos depois de meses bem bonita só abrindo netflix https://t.co/ac0gmsakce</t>
+  </si>
+  <si>
+    <t>saudades de station 19, cadê as temporadas netflix... até pouco tempo só tinha a 1ª 🥺 https://t.co/s8qk9p5ccg</t>
+  </si>
+  <si>
+    <t>@foioguto algum dia vc vai fazer um video sobre gokushufudou? ele é um manga mas 8 de abril lança o anime na netflix</t>
+  </si>
+  <si>
+    <t>tô chorando até agora com a eunyoo descobrindo q o irmão tava mentindo e que ela não ia voltar nunca vou superar e se ele não voltar na 2° temporada eu me mato e coloco a culpa na netflix https://t.co/cwc0yzkvpw</t>
+  </si>
+  <si>
+    <t>@beastarsbrasil não é atoa que o anime é da netflix</t>
+  </si>
+  <si>
+    <t>lembrei de quando achei um diário no meio de uns livros usados. as passagens icônicas. as brigas com o namorado. os dramas familiares. os perrengues com dinheiro. todo o arco do início da vida adulta retratados. melhor que muita série da netflix.</t>
+  </si>
+  <si>
+    <t>alô netflix favor colocar a última temporada de the 100 no catálogo, todo mundo já assistiu menos eu kkk</t>
+  </si>
+  <si>
+    <t>esse filme da netflix é mto bom amay o final pqp</t>
+  </si>
+  <si>
+    <t>meu sonho se a netflix fizesse um filme sobre mitologia grega.</t>
+  </si>
+  <si>
+    <t>esse filme silenciadas da netflix 
+pica demais né amei</t>
+  </si>
+  <si>
+    <t>mds o tanto de dorama que tem na minha lista da netflix que ódio</t>
+  </si>
+  <si>
+    <t>mais uma série que terminei em dois dias e a netflix vai cancelar ela daqui uns tempo quer apostar quanto 😹</t>
+  </si>
+  <si>
+    <t>comédia policial à brasileira, “cabras da peste” estreia na netflix https://t.co/4hy4mnv5mk</t>
+  </si>
+  <si>
+    <t>atinys vão no link nesse tweet e coloquem como sugestão:
+"imitation 이미테이션 by kbs2" 
+em seguida envie, vc n precisa ter uma conta pra  poder fazer a sugestão, vamos por imitation na netflix! @ateezofficial https://t.co/jk66klvolo</t>
+  </si>
+  <si>
+    <t>phoebe dynevor, a estrela da primeira temporada da série da netflix "bridgerton", vai ser a estrela de "the colour room". https://t.co/hlw2etgamu</t>
+  </si>
+  <si>
+    <t>@maytwita netflix. é uma série de investigação de estupros</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix bem q poderia soltar a data da 5b no meu aniversário https://t.co/w1zbdvu6pj</t>
+  </si>
+  <si>
+    <t>tava pensando em dividir netflix com alguém, mas agora q vou ter aula, essa ideia seria mais um gatilho pra minha procrastinação</t>
+  </si>
+  <si>
+    <t>eu só quero um pouquinho de serotonina e a única pessoa que pode me dar isso é a @netflix com a segunda temp de julie and the phantoms</t>
+  </si>
+  <si>
+    <t>@netflixbrasil boa tarde netflix lança a terceira temporada de you pelo amor de deus</t>
+  </si>
+  <si>
+    <t>aff, fui assistir todos os filmes da saga de velozes e furiosos antes da netflix tirar da plataforma e definitivamente eu nunca superei a morte do paul walker, parece que eu era próxima dele do tanto que eu sofro, vou ficar bad o dia todo por isso, o cara era a alma dos filmes</t>
+  </si>
+  <si>
+    <t>@abrahamweint @pbial hoje vai chamar a @majucoutinho para explicar o porquê o choro é livre, por favor, alguém me conte como foi... ficção eu prefiro a netflix
+@globonews @redeglobo @jornalbsm @tercalivre @taoquei1 @biakicis @carlazambelli38 @brasil_paralelo @brasilparalelo @jairbolsonaro</t>
+  </si>
+  <si>
+    <t>@_animese meu deus jojo na netflix eu precisa disso</t>
+  </si>
+  <si>
+    <t>@xacundim mas como ninguém tava falando dele antes olha a sinopse disso parece super divertido eu vou ver mais tarde (se meu netflix roubado ainda funcionar)</t>
+  </si>
+  <si>
+    <t>netflix anuncia série espanhola no brasil, “santo”, com bruno gagliasso - https://t.co/8nlkprvdax</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa que alina starkov é a maior!</t>
+  </si>
+  <si>
+    <t>noah cameron schnapp é um ator norte-americano, mais conhecido por interpretar will byers na série de televisão stranger things da netflix e dar voz a charlie brown no filme the peanuts movie. está também em um novo filme chamado hubie halloween também da netflix.</t>
+  </si>
+  <si>
+    <t>estréia do dia #netflix
+b: the beginning (2º temporada)
+"o genial investigador keith flick regressa à policia bem quando o serial killer “b” entra em ação. o misterioso jovem koku pode ser um aliado. ou será ele um alvo?" https://t.co/bv0zujcfnk</t>
+  </si>
+  <si>
+    <t>estréia do dia #netflix
+cabras da peste (2021)
+"dois policiais azarados se deparam com bandidos perigosos enquanto procuram a adorada cabra celestina. será que vai dar bode?" https://t.co/ttg2kpxzok</t>
+  </si>
+  <si>
+    <t>@darcypoeisy netflix ridícula tirou do catálogo 😭</t>
+  </si>
+  <si>
+    <t>quando teremos um documentário do bts na netflix pra eu poder usar icon do yoongi</t>
+  </si>
+  <si>
+    <t>me indiquem filmes clichês na netflix</t>
+  </si>
+  <si>
+    <t>@tto____wyu eu comecei faz pouco, foi numa madrugada de 2018, eu vi caramelldansen no youtube e queria ver algo visualmente igual, daí eu achei madoka na netflix asdfhbgj</t>
+  </si>
+  <si>
+    <t>@luvkilluaz yaas é perfeito
+tem na netflix assisto logo</t>
+  </si>
+  <si>
+    <t>não perdoo a netflix queria muito saber como iria ficar sterling e april e como a família ia ficar com os 838338 segredos</t>
   </si>
   <si>
     <t>sobre relacionamentos 
@@ -883,315 +671,55 @@
 curte que eu mando</t>
   </si>
   <si>
-    <t>finalmete algo interessante né netflix?
-só para variar https://t.co/95fwd2uewc</t>
-  </si>
-  <si>
-    <t>eu estava sem nenhuma série pra assistir e achei na netflix e me interessei we love you kyndra https://t.co/b6cjfzzfko</t>
-  </si>
-  <si>
-    <t>essa série que a netflix lançou polos opostos é tão ruim meu deus perdi meu tempo</t>
-  </si>
-  <si>
-    <t>nao consigo tirar print da netflix, q cu</t>
-  </si>
-  <si>
-    <t>parece um trailer de série da netflix e eu amei?????????????????????????
-de verdade, achei gostosinho. já quero! https://t.co/uk2eqzz4gt</t>
-  </si>
-  <si>
-    <t>@jessica16586798 @joongkibrazil oi boa tarde tem outro lugar que eu possa ver vincenzo  pq não tenho netflix</t>
-  </si>
-  <si>
-    <t>num mundo onde extise futebol
-futebol americano
-vôlei 
-futevolei 
-netflix
-amazon prime video
-disney plus
-o camarada vai assistir basquete kskskskkskskskks 10 nego tentando jogar um bola numa cesta kskskkssks tnc https://t.co/izvrcngaph</t>
-  </si>
-  <si>
-    <t>eu odeio a netflix que ódio</t>
-  </si>
-  <si>
-    <t>acabei de terminar de assistir na netflix o filme "mestres do yin-yang o sonho da eternidade" eu gostei bastante mais buguei muito com o plot twist, não que seja algo muito absurdo é que to meio lesado mesmo kkkkk</t>
-  </si>
-  <si>
-    <t>vao tirar the witch pq netflix me explique agr https://t.co/wh2oqy2kn0</t>
-  </si>
-  <si>
-    <t>@jelssreboucas se eu assistir oq assisto na netflix a véia morre do coração kkk me resta assistir globo né</t>
-  </si>
-  <si>
-    <t>@lelerosam só a melhor produção da netflix</t>
-  </si>
-  <si>
-    <t>quarto tá geladinho, vou me internar na netflix, não coloco a cara na rua hoje</t>
-  </si>
-  <si>
-    <t>será que a netflix vai lançar incon da série de grisha???? aaaaaaaansiosaaaaaaa</t>
-  </si>
-  <si>
-    <t>poha netflix lança logo a segunda temporada de sintonia aí</t>
-  </si>
-  <si>
-    <t>finalmente o filme do dylan vai entrar na netflix 🙏🏼🙏🏼🙏🏼</t>
-  </si>
-  <si>
-    <t>@worstthingsfx perdão amigo mas o cinema acabou durante a pandemia e só sobrou netflix originals</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. não 
-2. 2
-3. leão 
-4. não 
-5. apegada
-6. no
-7. depende 
-8. é complicado, mas solteira
-9. jantar fora
-10. netflix em casa
-11. acredito
-12. não 
-13. não 
-curte que eu mando</t>
-  </si>
-  <si>
-    <t>filme na netflix com meus amores🥰❤</t>
-  </si>
-  <si>
-    <t>@blaxyves @ryjndy eu sou um partidão tá ia fazer cafuné o tempo todo, ia levar lanchinho no trabalho, mandar mensagens fofinhas dizendo o quanto é importante, dar o login das minhas plataformas (netflix, amazon prime, globoplay e disney plus) e dar coisinhas do red velvet
-mas ngm me dá uma chance</t>
-  </si>
-  <si>
-    <t>nem pra marvel olhar para os oprimidos e colocar a série do loki na netflix e não no disney+😔😔</t>
-  </si>
-  <si>
-    <t>que venha 
-mas to surpresa pq não é do feitio da netflix soltar trailer um mês antes https://t.co/myxg3ktrhf</t>
-  </si>
-  <si>
-    <t>novo conceito de romance da netflix: rolê na funerária, ouvir musiquinha deitados dentro de um caixão 
-gostei vou aderir</t>
-  </si>
-  <si>
-    <t>netflix caralho vai renovar jatp quando porraaaaaa</t>
-  </si>
-  <si>
-    <t>@pmanupe aparentemente: pegarlle aos escravos por aburrimento &amp;gt;&amp;gt;&amp;gt;&amp;gt; ver netflix</t>
-  </si>
-  <si>
-    <t>@wfoxmoon deve ser amg pq meu deus kkkkkkkk
-fora q a netflix tb vem com uns nomes nada ver</t>
-  </si>
-  <si>
-    <t>af só queria estar namorando pra dizer, ei vida sexta lá em casa, vinho, pizza, netflix, sem muita burocracia</t>
-  </si>
-  <si>
-    <t>@sun__nyu sim eu também 
-se netflix cancelou as séries pra fazer esses efeitos eu até dou um desconto</t>
-  </si>
-  <si>
-    <t>@marbundas a mulher não da ponto sem nó amigo 🗣🗣🗣 e a lenda ainda tá riquíssima agora empregada pela netflix</t>
+    <t>chuvinha boa pra deita na cama e liga a netflix</t>
+  </si>
+  <si>
+    <t>@cowidflys2 netflix. chama “por trás de seus olhos”</t>
   </si>
   <si>
     <t>@vaidezete já deitei uma parte, falta o resto mas quero ter certeza q tô deitando e n só me prejudicando gostando de artista ent pra eu ter certeza vou ver oq vc falou lá na netflix</t>
   </si>
   <si>
-    <t>que tristeza ver como o nível dos filmes caiu tanto. os indicados ao oscar, muitos na grade da netflix, são filmes que não merecem estar na sessão da tarde.</t>
-  </si>
-  <si>
-    <t>por favor assistam "meu nome é ray" tem na netflix</t>
-  </si>
-  <si>
-    <t>@ririrwilliams pena que saiu da netflix 😢 eu assistia todo ano
-agora tenho preguiça de baixar todas as temporadas mas morrendo de saudade</t>
-  </si>
-  <si>
-    <t>@netflixbrasil ela precisa ser a américa de a seleção. tá ouvindo netflix????</t>
-  </si>
-  <si>
-    <t>alguem de bom coração quer dividir a netflix comigo</t>
-  </si>
-  <si>
-    <t>alguém sabe onde eu posso assistir o documentário "cosmos"? ja que a netflix nos fez o favor de tirar do site</t>
-  </si>
-  <si>
-    <t>um romance água com açúcar que envolve patinação e hockey???? netflix te amo</t>
-  </si>
-  <si>
-    <t>@doougfuny to na expectativa ja e amanhã ainda sai tbm aquela da formula 1 na netflix. bastante coisa pra maratonar. hahahaha
-ah e o snyder cut nem animei, 4h é muito num filme. hahahahah</t>
-  </si>
-  <si>
-    <t>que saudade do meu reality @thecirclebra 
-alô alô netflix cadê a segunda temporada</t>
-  </si>
-  <si>
-    <t>@eii_thyyleite_ mas a netflix mesmo assim continua renovando um monte de série</t>
-  </si>
-  <si>
-    <t>amo aassistir o show  da taylor que tem na netflix</t>
-  </si>
-  <si>
-    <t>🚨 tentativa de interação
-qual a melhor série da netflix na opinião de vcs?</t>
-  </si>
-  <si>
-    <t>vamos assistir sessão da tarde, já que eu não tenho wi-fi pra ver netflix.</t>
-  </si>
-  <si>
-    <t>@floweredstorm só deixaram três na netflix acredita sabs e nem é qual que eu gosto😭😭😭</t>
-  </si>
-  <si>
-    <t>@gfb_grp na netflix só tem até a 17</t>
-  </si>
-  <si>
-    <t>@harlancoben @stayclosehc @realmikefox @murderbooks estou assistindo safe on netflix 👏🏼👏🏼👏🏼série maravilhosa.. @harlancoben um grande escritor!!!</t>
-  </si>
-  <si>
-    <t>amanhã na netflix é tudo q eu preciso 🥲 https://t.co/anjcbeblu8</t>
-  </si>
-  <si>
-    <t>alou, f1tt 📢📢 🏁
-querem uma sugestão de série curtinha e engraçada pra maratonar antes de dts 3? 
-the crew foi lançada em 2021 pela netflix e é uma sitcom que retrata o dia a dia de uma equipe mediana da nascar. é estrelada pelo kevin james e o freddie stroma. https://t.co/ze7iqhvo5x</t>
-  </si>
-  <si>
-    <t>@enelparadinight @kanoh_agitobr @liposochan @ferkinghill @netflixbrasil acho que so vai acontecer de skypiea ser lançada na netflix.</t>
-  </si>
-  <si>
-    <t>@abrahamweint @pbial hoje vai chamar a @majucoutinho para explicar o porquê o choro é livre, por favor, alguém me conte como foi... ficção eu prefiro a netflix
-@globonews @redeglobo @jornalbsm @tercalivre @taoquei1 @biakicis @carlazambelli38 @brasil_paralelo @brasilparalelo @jairbolsonaro</t>
-  </si>
-  <si>
-    <t>@lloudete a netflix teria monte de conteudo para fazer séries, aq no fandom da loud</t>
-  </si>
-  <si>
-    <t>descobri q tem na netflix, esse eh o motivo do meu colapso https://t.co/e3p31mvact</t>
-  </si>
-  <si>
-    <t>@_animese @sifudemalucoo @ashhtalented é isso mesmo que eu li????? jojo na netflix??? agora todo mundo vai conhecer essa obra prima 👌🏻</t>
-  </si>
-  <si>
-    <t>eu compartilho o netflix com um monte de gente ai pedi pras mesmas me emprestar outras plataformas e falaram q não da ou mudaram de assunto</t>
-  </si>
-  <si>
-    <t>bruno gagliasso estreia em santo, série original espanhola da netflix https://t.co/emdtdi2r8t</t>
-  </si>
-  <si>
-    <t>caraca n tem uma serie na netflix q me prenda</t>
-  </si>
-  <si>
-    <t>essa linda e eterna paixão de clary e jace @kat_mcnamara @domsherwood1 não pode dizer adeus ao meu coração #shadowhunters #saveshadowhunters #clace #jaceherondale #claryfairchild @constantinfilm @netflix @thecw https://t.co/jw7tgn4tuc</t>
-  </si>
-  <si>
-    <t>@ale_eufrasio @brlalita_ @lalifasbr @netflixbrasil @esposbrasil a gente tá tendo fazer o mínimo que a netflix br não tá fazendo, por isso que a gente estava aqui no twitter da netflix br pedindo divulgação</t>
-  </si>
-  <si>
-    <t>@ale_eufrasio @lalifasbr @netflixbrasil @esposbrasil não dá conta? então quer dizer que você reclama com todo mundo que pede pra netflix renovar jatp, que pede lucifer, que pede pra renovar sei lá o que? putz</t>
-  </si>
-  <si>
-    <t>irritada pq desde que divergente saiu na netflix e virou modinha o povo começou a ficar obcecado com o theo james e eu sou apaixonada nele e nos livros desde 2014 🤬</t>
-  </si>
-  <si>
-    <t>aí tava vendo "professor iglesias(netflix)" e um aluno preto dele disse assim:
-"vc sabe de como é dificil ser considerado um homem preto muito bonito hoje em dia? o michael b jordan elevou a barra à um nível inalcançável." https://t.co/gdq6llfm07</t>
-  </si>
-  <si>
-    <t>netflix anuncia série espanhola com bruno gagliasso  https://t.co/haxyykdvmi</t>
-  </si>
-  <si>
-    <t>🎥hollywood | ryan murphy e ian brennan (2020)
-logo após a 2ª guerra mundial, hollywood atrai jovens atores, roteiristas e diretores dispostos a enfrentar barreiras étnicas, de gênero e sexualidade, mantidas até então pela elite cinematográfica. (netflix)</t>
-  </si>
-  <si>
-    <t>a netflix assustou a galera que compartilha senhas, enviando um "aviso" para alguns usuários. acho pouco provável que uma mudança grande aconteça. todo mundo compartilha senhas, todo mundo (a própria netflix, inclusive) sabe disso e… está tudo bem?
-https://t.co/pccrb5ctkt</t>
-  </si>
-  <si>
-    <t>se a netflix colocar jojo começando pela parte 3 eu explodo aquela empresa</t>
+    <t>pra esse dia friozinho, café, netflix e moletom 🤍</t>
+  </si>
+  <si>
+    <t>@suwastann erased, tem na netflix e tem 13 eps
+é um dos meus favs e tem plot twist na historia</t>
+  </si>
+  <si>
+    <t>vc vai fazer oq final de semana? — assistir netflix, chorar e dormir  https://t.co/whccogncde</t>
+  </si>
+  <si>
+    <t>@luishenriqueu se for é por causa da netflix com essas produções baratas aí</t>
+  </si>
+  <si>
+    <t>@arima_lib sandman é demais, nunca li nenhum hq melhor
+o q me deixa com um pé atrás é eles estarem com a netflix, mas nao vou desistir só por causa disso, eles vão fazer jus àquele universo, queira deus</t>
+  </si>
+  <si>
+    <t>assistam pose na netflix. só isso.</t>
+  </si>
+  <si>
+    <t>@bayerniludido eu criando 24 fakes pra ver netflix de graça pra sempre</t>
+  </si>
+  <si>
+    <t>#netflix testa função para impedir compartilhamento de senhas. vem ver: https://t.co/b7anmmkoid https://t.co/i9rcoliaqz</t>
   </si>
   <si>
     <t>@emotacokkkk @op_netflix_fan @kkluisui hiriluk entre na minha casa e cure toda minha família</t>
   </si>
   <si>
-    <t>aí queria só um conta da netflix</t>
-  </si>
-  <si>
-    <t>pela aba de em breve da netflix (ficou na minha lista por tipo um mês e dps comecei a ver fotos no instagram delas e comecei a assistir)
-we love you kyndra https://t.co/wqqqf3jo2l</t>
-  </si>
-  <si>
-    <t>pq q essas série boa tem que ter só uma temporada ????porra netflix eu preciso de mais</t>
-  </si>
-  <si>
-    <t>sim amiga o hamilton só vai ter 5 minutos no dts pq a netflix n quis fazer com ele, com toda certeza não foi porque ele foi pela saco pelo terceiro ano seguido e não quis gravar pra equipe dos caras</t>
-  </si>
-  <si>
-    <t>por deus i land é a pior serie que eu ja vi na vida netflix como vc teve coragem de fazer uma coisa dessaskkkkkkkkkkkkkk patetico</t>
-  </si>
-  <si>
-    <t>chegou meu almanaque da netflix @netflixbrasil tu serviu viu fia</t>
-  </si>
-  <si>
-    <t>@manuriosnotice @jsantos455 tá todo mundo pedindo o hot deles @netflix</t>
-  </si>
-  <si>
-    <t>@vicionerd16 
-agora que jojo vai inteiro pra netflix
-será que sai dublagem? https://t.co/hxfecg1llk</t>
-  </si>
-  <si>
-    <t>encontrei um video na netflix da barbie e do ken cantando parabéns pra vc, n sei como reagir</t>
-  </si>
-  <si>
-    <t>por aqui vendo uma netflix 🙄</t>
-  </si>
-  <si>
-    <t>tanto anime bom pra botar no catálogo e a netflix vai botar jojo</t>
-  </si>
-  <si>
-    <t>@izzatarts @bellekaffer tu por acaso só olha anime na netflix? kkkk</t>
-  </si>
-  <si>
-    <t>do que adianta ter netflix, prime video, globoplay e disney+ se nenhum deles tem os filmes da barbie?</t>
-  </si>
-  <si>
-    <t>@dougxss tem uma série na netflix parecida chama-se 
-perfume</t>
-  </si>
-  <si>
-    <t>tem mts pessoas que estão esperando a segunda temporada e a @netflixbrasil
-@netflix
-ficam de palhaçada sem renovar a série 😤
-aaaah eu amo 😍
-#julieandthephantoms eu só queria a segunda temporada 🙁</t>
-  </si>
-  <si>
-    <t>e vamos de "as loucuras de dick &amp;amp; jane" na netflix!
-https://t.co/nndd6kvzsf</t>
-  </si>
-  <si>
-    <t>fui ver o filme novo da netflix e só confirmei que eu realmente não gosto de criança pqp</t>
-  </si>
-  <si>
-    <t>chuvinha boldo do bom, netflix e pipoca= tarde perfeita</t>
-  </si>
-  <si>
-    <t>tô chorando até agora com a eunyoo descobrindo q o irmão tava mentindo e que ela não ia voltar nunca vou superar e se ele não voltar na 2° temporada eu me mato e coloco a culpa na netflix https://t.co/cwc0yzkvpw</t>
-  </si>
-  <si>
-    <t>✨ divulgado um novo teaser trailer de "sombra e ossos", nova série da netflix que estréia no dia 23 de abril.
-#shadowandbone 
-https://t.co/il8k8g8ulo</t>
-  </si>
-  <si>
-    <t>@filmesdochico “saint maud” vc deve ter visto...... 
-“m-8”, nacional na netflix. apesar de ter umas fraquezas, achei a execução, o roteiro e os subtextos raciais, classe, muito bons. fiquei muito gratamente surpreso.</t>
+    <t>netflix: vocês ainda estão assistindo?
+nós dois: https://t.co/fq1tu835ft</t>
+  </si>
+  <si>
+    <t>quais são os melhores doramas que tem na netflix?</t>
+  </si>
+  <si>
+    <t>netflix tava cim a faca e o queijo na mão pra fazer uma serie enemies to lovers um jogador de hoquei marmanjo e uma patinadora artística e ai eles tem que patinad juntos e acabam se apaixonando mas nessa serie polos opostos parece q eles sao irmaos</t>
+  </si>
+  <si>
+    <t>@op_netflix_fan @hahiyos isso ta melhor q minha visão</t>
   </si>
   <si>
     <t>oferta 2021 abençoado | 30% off
@@ -1203,115 +731,69 @@
 #arsenelupin #livrariacristaemmerick #mauriceleblanc #lupin #netflix https://t.co/b64vhwgmv3</t>
   </si>
   <si>
-    <t>@nalaurachiq tem um na netflix de uma assassina, não lembro se tem festa, mas tem vestido chique ava o nome</t>
-  </si>
-  <si>
-    <t>eu não lembro direito, eu acho que vi alguém na tml falando e dps apareceu no catálogo da netflix pra mim 
-we love you kyndra https://t.co/5w5z1biu9j</t>
-  </si>
-  <si>
-    <t>como é que a netflix tem doze homens e outro segredo e doze homens e um outro segredo, mas não tem doze homens e um segredo? vtc</t>
-  </si>
-  <si>
-    <t>@netflixbrasil uai, não vai lançar a próxima parte lúcifer não netflix??!! poxa</t>
-  </si>
-  <si>
-    <t>apareceu na minha netflix e eu comecei a ver 
-we love you kyndra https://t.co/qixovsn40p</t>
-  </si>
-  <si>
-    <t>como caralho a netflix não gravou a corrida do 7° título do hamilton e o pódio do vettel 😭😭😭😭</t>
-  </si>
-  <si>
-    <t>porra minha tl tá lotada com pedro pedindo a porra do dragon ball pra netflix q ódio viu</t>
-  </si>
-  <si>
-    <t>@crowylies ah isso? fiquei puta por conta pela falta dos outros personagens mas honestamente? o que esperar da netflix?</t>
-  </si>
-  <si>
-    <t>não aguento mais minha netflix sendo hackeada</t>
-  </si>
-  <si>
-    <t>hj era o dia perfeito para ficar assistindo netflix com elaaaaa🥺😕 @fabolavitria7 tendeu?</t>
-  </si>
-  <si>
-    <t>ele já fez o filme todo de teste é só a netflix chamar https://t.co/tgty8prvpf</t>
-  </si>
-  <si>
-    <t>só queria ela e a netflix agora</t>
-  </si>
-  <si>
-    <t>tava lendo sobre as chaves que não apareceram na série e pelo amor de deus netflix me de a chave harleyquinn</t>
-  </si>
-  <si>
-    <t>trad: atinys! para dar ao @ateezofficial mais exposição nacional e internacionalmente, acesse este link (para sugestões de programas de tv da netflix)
-🔗: https://t.co/6s850ejwsa
-e digite "imitation 이미테이션 by kbs"
-quando terminar, envie sua sugestão. muito obrigado! https://t.co/utcz7ali7r</t>
-  </si>
-  <si>
-    <t>@only_fe_ tô assistindo na netflix msm :(</t>
-  </si>
-  <si>
-    <t>na moral mas o wylan é muito esquecido pela netflix cara, eles mudam bastante coisa dos crows, dava pra arranjar um modo de já colocar o garoto nessa season, msm que com uma participação pequena, mas eles só ligam pra jesper, kaz e inej 😭😭😭</t>
-  </si>
-  <si>
-    <t>e teve um dia que a tv da sala ligou as 03h da manhã eu estava ouvindo vozes e não sabia o que era ai eu fui ver e a tv tava ligada (realidade: meu vizinho conectou a netflix na minha tv e ela ligou sozinha mesmo estando desligada) eu tranquei o cu</t>
-  </si>
-  <si>
-    <t>pq a netflix faz série com 1t e 9ep p gente acabar rápido e ficar sofrendo esperando 5 anos pelo resto?!?!? oh ódio viu</t>
-  </si>
-  <si>
-    <t>galera, segunda temporada de love alarm 
-como eu n lembro nada da primeira kkkkk torci p hye-yeong
-mas serio, foi muito parada, exploraram pouquissimo os personagens, senti sono 75% do tempo
-to decepcionada, dona netflix.
-atores bons
-primeira temporada boa
-tinha a faca e o queijo</t>
-  </si>
-  <si>
-    <t>comédia policial à brasileira, cabras da peste estreia na netflix. veja mais em: tribuna do sertão - https://t.co/d2amgr9gwb</t>
-  </si>
-  <si>
-    <t>eu amo um clichê familiar obrigada netflix</t>
-  </si>
-  <si>
-    <t>@viitey os cara tão enchendo seu saco ainda por causa do post de jojo na netflix?</t>
-  </si>
-  <si>
-    <t>aff, fui assistir todos os filmes da saga de velozes e furiosos antes da netflix tirar da plataforma e definitivamente eu nunca superei a morte do paul walker, parece que eu era próxima dele do tanto que eu sofro, vou ficar bad o dia todo por isso, o cara era a alma dos filmes</t>
-  </si>
-  <si>
-    <t>me recomendem algo pra assistir na netflix, mutuals</t>
-  </si>
-  <si>
-    <t>🎬12 - cena do crime - mistério e morte no hotel cecil | 2020
-• diretor: joe berlinger
-• gênero: documentário
-• netflix studios
-⭐️⭐️⭐️ https://t.co/y1tclctwdd</t>
-  </si>
-  <si>
-    <t>mamãezinha que trabalha para netflix e amazon prime ao mesmo tempo https://t.co/sujceffo4k</t>
-  </si>
-  <si>
-    <t>eu menti para você, não tenho netflix, tampouco vamos transar. vamos assistir filme de super herói regravado com mais de 4h de duração</t>
-  </si>
-  <si>
-    <t>puta merda @netflix pukê puuukê você fez esse final de #lovealarmseason2 eu tava na esperança maaaan</t>
-  </si>
-  <si>
-    <t>eu deitado na minha cama, netflix na tv</t>
-  </si>
-  <si>
-    <t>é verdade que a netflix não vai mostrar o gp da turquia??</t>
-  </si>
-  <si>
-    <t>@omelhorluiz @netflix te marquei? https://t.co/kmzzcjmgmo</t>
-  </si>
-  <si>
-    <t>meu sonho se a netflix fizesse um filme sobre mitologia grega.</t>
+    <t>preciso de uma 2 temporada de ginny e georgia netflix</t>
+  </si>
+  <si>
+    <t>eu nem tenho mais oq ver na netflix q saco</t>
+  </si>
+  <si>
+    <t>sozinho d cs, fumando um kank vendo netflix 😅🍁</t>
+  </si>
+  <si>
+    <t>queria que a netflix só n tivesse divulgado o ator do wylan mas na real ele tá na série daí eu estaria assistindo e do nada “pah o wylan” seria muito emocionante mas sei que n passa de um sonho 😔</t>
+  </si>
+  <si>
+    <t>netflix, academia, desenhar, sair com os amigos... basicamente nada mais me deixa alegre... https://t.co/3v8y0jqfmu</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix me prometa que expresso do amanhã vai ter mais uma temporada</t>
+  </si>
+  <si>
+    <t>@bergaraujosilva vc ja viu o filme dela no netflix?</t>
+  </si>
+  <si>
+    <t>@netflixbrasil @netflix vou entrar em depressão sério</t>
+  </si>
+  <si>
+    <t>vai lançar damon slayer na netflix, vou assistir pela tv 😍</t>
+  </si>
+  <si>
+    <t>@denkicelest sweet home é um terro bem daora mais é bem pesado tem gore 
+tem la no netflix</t>
+  </si>
+  <si>
+    <t>@_chei a série está em pre-produção pelo netflix, com produção do filho do gabriel garcia marques</t>
+  </si>
+  <si>
+    <t>jojo e kimetsu no yaiba vão entrar na netflix agora eu quero saber quando vai entrar haikyuu</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estrelará série espanhola de ação da netflix https://t.co/tqbrzcsdxe</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix a seleção é real ou lenda urbana?</t>
+  </si>
+  <si>
+    <t>@henriquethe2 eita, ela estava na mira da netflix</t>
+  </si>
+  <si>
+    <t>sobre relacionamentos 
+1. hoje não. 
+2. que eu saiba foram 4.
+3. não preciso de outro, com o meu já faço isso.
+4. dizem que sim.
+5. achava que era desapegado, mas mais uma vez fazendo papel de palhaça.
+6. hoje não faro.
+7. nao
+8. namorando
+9. jantar fora.
+10. netflix 
+11. não.</t>
+  </si>
+  <si>
+    <t>alou, f1tt 📢📢 🏁
+querem uma sugestão de série curtinha e engraçada pra maratonar antes de dts 3? 
+the crew foi lançada em 2021 pela netflix e é uma sitcom que retrata o dia a dia de uma equipe mediana da nascar. é estrelada pelo kevin james e o freddie stroma. https://t.co/ze7iqhvo5x</t>
   </si>
   <si>
     <t>vai gringa, surta mais pq não quer seu fav na netflix, que saco vcs querem ver eles desempregados ou o que? disney? nao pode
@@ -1319,352 +801,356 @@
 gente?? eles precisam trabalhar e botar coisa no currículo, ator que recusa papel não ganha dinheiro</t>
   </si>
   <si>
-    <t>eu só queria shameless us na porra da netflix ou pelo menos em algum outro canal de streaming pq mds cansado de tentar conseguir baixar isso</t>
-  </si>
-  <si>
-    <t>porra vários animes que vai entrar na netflix. agora tá dando gosto de pagar essa bosta</t>
-  </si>
-  <si>
-    <t>roteiro melhor q dos filmes da netflix</t>
-  </si>
-  <si>
-    <t>assistam irmandade, sério 
-assistam é simplesmente a melhor serie da netflix feita! https://t.co/vzbqqq6qfc</t>
-  </si>
-  <si>
-    <t>e hj que descobrir que no meu plano de celular, tenho netflix e yt “grátis”, já faz 1 ano e fui saber hj aiai</t>
-  </si>
-  <si>
-    <t>@netflixbrasil @esposbrasil ué netflix mas você não tá divulgando mesmo kkkkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>imagens chocantes:
-veja como está o tom holland após ser demitido pela marvel e pela netflix. https://t.co/dz7l1skrn0</t>
-  </si>
-  <si>
-    <t>@xacundim mas como ninguém tava falando dele antes olha a sinopse disso parece super divertido eu vou ver mais tarde (se meu netflix roubado ainda funcionar)</t>
-  </si>
-  <si>
-    <t>@ness4richards amg tem alguns “”spin offs”” de equestria girls, e algumas temporadas de my little pony, antes tinhas os filmes, mas a netflix tirou</t>
-  </si>
-  <si>
-    <t>@andremans mano, eu dei like nesse tuite pra eu poder procuar o filme depois... no fim, nao tem na netflix daqui :(</t>
-  </si>
-  <si>
-    <t>todos nós juntos somos mais fortes e vamos continuar lutando pela volta da nossa linda série #shadowhunters #saveshadowhunters @constantinfilm @netflix @thecw @shadowhunterstv https://t.co/nuhpgggjeb</t>
-  </si>
-  <si>
-    <t>netflix fazendo segunda temporada pra um anime de 2017 e portanto me obrigando a assistir as duas visto que eu não lembro de nada que tenha ocorrido já mais de 7 dias</t>
-  </si>
-  <si>
-    <t>@stf_oficial quem vai me obrigar ir no cinema assistir porcaria, baixei alguns no netflix não gostei, deletei, procuro selecionar, não é qualquer porcaria que assisto, simples assim, para de interferir em nossas escolhas. prisão em 2ª instância é mais importante para ficarmos livre do lula.</t>
-  </si>
-  <si>
-    <t>@sitor_vilveira meu deus é da netflix*** kkkkkkkkkkk pane no sistema</t>
-  </si>
-  <si>
-    <t>eu ainda nao superei esse encontro seu jorge e jason momoa, netflix eu deixei em suas maos juntar esse dois num filme e me fazer feliz</t>
-  </si>
-  <si>
-    <t>teoricamente nós temos até março do ano que vem pra assistir a terceira temporada.
-eu escolhi esperar. (até arrumar dinheiro pra assinar a netflix 😔) https://t.co/ucaxo7kerx</t>
-  </si>
-  <si>
-    <t>tava quase na deep web tentando achar o anime pra baixar, fui ver tem na netflix 🤡</t>
-  </si>
-  <si>
-    <t>a
-percebi agora que colocar mais anime na netflix vai estragar muitas fandoms...
-to com medo agora</t>
-  </si>
-  <si>
-    <t>netflix tinha que parar de lançar série nova e começar a lançar as temporadas novas das séries que estão paradas há tempos</t>
-  </si>
-  <si>
-    <t>@camilly_tr entendiii bb ! tava c netflix e amazon aí cancelei a netflix mantive só a amazon , mas tava querendo ver uma dessas aí globo play ou telecine</t>
-  </si>
-  <si>
-    <t>ainda não me desceu essa idiotice do "choro é livre" da #calaabocamajuhipocrita 
-as pessoas que trabalham para sustentar a família tb queriam ter salário alto da #globolixo @redeglobo e ficar em casa assistindo globoplay ou netflix. mas nem td mundo tem sorte de viver de lacração https://t.co/a1rezd0cxi</t>
-  </si>
-  <si>
-    <t>preciso ter você @domsherwood1 junto do meu coração #shadowhunters #saveshadowhunters #jaceherondale @constantinfilm @netflix @thecw https://t.co/c2kkrst4af</t>
-  </si>
-  <si>
-    <t>netflix sua puta pq não coloca haikyuu?????? https://t.co/dttmdckiuc</t>
+    <t>@gabrioches @op_netflix_fan que coisa mais linda</t>
+  </si>
+  <si>
+    <t>como caralho a netflix não gravou a corrida do 7° título do hamilton e o pódio do vettel 😭😭😭😭</t>
+  </si>
+  <si>
+    <t>@carlasv17 com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>meus app tão tudo na merda, zap num funciona, meu dd no insta nem entra, a netflix n carrega, mais q saco</t>
+  </si>
+  <si>
+    <t>@tayaraandrade4 netflix amiga. 6 ep só, mto mto boa mesmo. amo finais surpreendentes</t>
+  </si>
+  <si>
+    <t>mesmo com uma série muito hypada o disney+ não consegue bater em uma série da netflix por causa do dobro de assinantes https://t.co/czfrp89psu</t>
+  </si>
+  <si>
+    <t>comédia policial à brasileira, cabras da peste estreia na netflix. #ndmais https://t.co/dcwqqpxtit</t>
+  </si>
+  <si>
+    <t>mds agr que percebi saiu do cartaz da netflix https://t.co/lsynnh2u2f</t>
+  </si>
+  <si>
+    <t>é fácil dizer isso, para quem vive numa bolha, salário em dia, geladeira cheia, um vinhozinho para relaxar à noite, vendo um filme na netflix.
+@majucoutinho https://t.co/8xoctngajb</t>
+  </si>
+  <si>
+    <t>não tem nenhuma série boa na netflix😭😭😭</t>
+  </si>
+  <si>
+    <t>o mesmo ator q fez um personagem de 30 anos em locke key interpretando um adolescente em ginny &amp;amp; georgia
+se isso n diz algo sobre as decisoes de cast da netflix kkkk</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix voce nao me da tempo nem de respirar que ja vem com lançamento</t>
+  </si>
+  <si>
+    <t>@joaopedrxfr kkkkkkkkkkkkkkkkkkkkkkkkkkkk vsfd bagulho ruim mano
+quando entrar na netflix eu vejo tudo mano prometo</t>
+  </si>
+  <si>
+    <t>meu deus eu criei um romance de netflix desisti de medicina vou virar escritor fodas @netflixbrasil se estiver interessada manda uma dm</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix coloca a era do gelo no catálogo eu nunca te pedi nada</t>
+  </si>
+  <si>
+    <t>vamo p terceiro filme de hoje, tô zerando a netflix no trampo kkk</t>
+  </si>
+  <si>
+    <t>se vc ainda não viu scissor seven e sangue de zeus na netflix, vc ta no erro</t>
+  </si>
+  <si>
+    <t>um monte de doce um monte de salgado e netflix, já estou resumindo meu final de semana.</t>
+  </si>
+  <si>
+    <t>o drive to survive (temporada 3) já está disponível na netflix?</t>
+  </si>
+  <si>
+    <t>@math_go2 assiste “o que você come” da netflix</t>
+  </si>
+  <si>
+    <t>imagina o filme de kimetsu saindo na netflix, eu só me relacionaria cm pessoas q assistissem esse filme cmg</t>
+  </si>
+  <si>
+    <t>@hhttnick dica de um conhecido do tt: assiste expresso do amanhã que cura tudo ( netflix )</t>
+  </si>
+  <si>
+    <t>@phytion1318 @_otakusbr questão da dublagem é com a própria netflix q contrata o estúdio, por isso n cabe ao estúdio ou os dubladores fazer isso por si só. mas depois da recepção positiva dos ova's tem chances q sim. mas como tá receber vamos esperar trailer de estará dublado ou n.</t>
+  </si>
+  <si>
+    <t>a netflix anunciou mais temporadas pra real housewives dia 15 de abril kct eu to nervosaaa</t>
+  </si>
+  <si>
+    <t>@egirldecorsa enquanto isso têm tantos talentos em busca de atuar e a netflix só escolhe os piores</t>
+  </si>
+  <si>
+    <t>esse video ficou 5 vezes melhor que o filme da netflix https://t.co/geizslu9jl</t>
+  </si>
+  <si>
+    <t>quinta é dia de tbt, hoje, falarei de initial d! você curte? comentarei ainda de kishibe rohan, anime spin-off de jojo na @netflix. será às 20h40, após funimation tv. até lá! #maisgeekloading https://t.co/y9o4kxtwth</t>
+  </si>
+  <si>
+    <t>q sdd de assistir the get down, jóinha rara da netflix</t>
+  </si>
+  <si>
+    <t>@_rodrigomattos_ qual a relação do futebol com a pandemia? os estádios estão com público? algum jogador esta infectado jogando? vai aglomerar em casa? então fecha o big bista e netflix, mandou o pvc</t>
+  </si>
+  <si>
+    <t>@srchances ve logo o anime da netflix
+so 10 eps
+rapidinho se acaba
+chorandp
+se lembre disso
+se acaba chorando</t>
+  </si>
+  <si>
+    <t>netflix: veja “código secreto” para encontrar documentários sobre crimes &amp;gt; https://t.co/1rgf1kq4pe https://t.co/kkarvsuaeg</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa que é ela</t>
+  </si>
+  <si>
+    <t>@renatobarrosbr com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>@netflixbrasil eu tenho tanta coisa pra fazer mas a netflix só fica lançando série e atrapalhando a minha vida affs...</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix ontem foi dia dos fãs e tu nem deu parabéns pros netflixers 
+(não vou te culpar porque eu só fiquei sabendo disso hoje kklsksk)</t>
+  </si>
+  <si>
+    <t>pensei que ia tirar o dia pra ver netflix mas infelizmente não deu,tenho que adiantar as matérias da faculdade...</t>
   </si>
   <si>
     <t>nossa vou cadelar gostoso nessa velha obrigada por tudo netflix https://t.co/3lsvplpv6g</t>
   </si>
   <si>
-    <t>@pieckkksimp @irismmonteiro aot tmb tem na netflix so n a ultima temp acho</t>
-  </si>
-  <si>
-    <t>acho engraçado que eu tenho amazon, netflix, disney +, globoplay mas não tenho coragem de assinar descomplica</t>
+    <t>@nikolas_dm com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>socorro eu li esse livro em 2013 e agr 8 anos dps vai virar serie na netflix https://t.co/ijyhqfv0xm</t>
+  </si>
+  <si>
+    <t>só minha netflix que tá bugada??? ódio</t>
+  </si>
+  <si>
+    <t>jamie foxx vive quatro personagens em nova série da netflix; veja trailer &amp;gt; https://t.co/zaeirxohim https://t.co/v9tewfofsp</t>
+  </si>
+  <si>
+    <t>meu deus, só tem homem nojento nessa série. o machismo, nos dias atuais, é uma coisa insuportável, imagina nos anos 60, onde a figura da mulher era associada a vida doméstica, que a violência sexual e física eram "normais" pra eles 🤮🤢
+#coisamaislinda #netflix</t>
+  </si>
+  <si>
+    <t>realmente essa série nova de piratas da netflix é um documentário encenado com baixo orçamento, mas não é ruim</t>
+  </si>
+  <si>
+    <t>@gfb_grp na netflix só tem até a 17</t>
+  </si>
+  <si>
+    <t>tava lendo sobre as chaves que não apareceram na série e pelo amor de deus netflix me de a chave harleyquinn</t>
+  </si>
+  <si>
+    <t>só queria ta deitadinha vendo um netflix f1 com as cias 😍🌈</t>
+  </si>
+  <si>
+    <t>@jessica_vrll por trás de seus olhos. 
+uma nova da netflix</t>
+  </si>
+  <si>
+    <t>vsf netflix br q ódio https://t.co/yppfgxi55v</t>
+  </si>
+  <si>
+    <t>netflix contrate agora, o maluco manja dos roteiros https://t.co/lultigcvy3</t>
+  </si>
+  <si>
+    <t>viciada em documentário sobre tecnologia 
+o código bill gates (netflix) é 10/10 e print the legend (netflix) também</t>
+  </si>
+  <si>
+    <t>@antoniobaggio8 @lembrancaspv @landonorrisbr @netflix chefe de cozinha é questionável pq já deixou algumas vezes a comida queimar 😂😂😂</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix mostra o trailer e eu digo se esperava ou não nunca te pedi nada mas já que tô pedindo vou aproveitar e pedir algum mimo de gentefied também beijo amor tenha uma tarde ótima</t>
+  </si>
+  <si>
+    <t>@gincanafriend avisa que é a série melhor da netflix</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix, sei que você é minha amiga, adianta algo ai de jupiter’s legacy e eu digo se esperava ou não</t>
+  </si>
+  <si>
+    <t>estréia do dia #netflix
+nate bargatze: the greatest average american (2021)
+"neste especial de comédia, nate bargatze fala sobre comédia pelo zoom, a perda de um celular, café da manhã de hotel, a nova matemática e muito mais." https://t.co/8eey7qcz6o</t>
+  </si>
+  <si>
+    <t>5 anos atrás eu era o rei da pirataria, olha oque a netflix fez comigo</t>
+  </si>
+  <si>
+    <t>queria indicações de filmes na netflix?🤔🙄</t>
+  </si>
+  <si>
+    <t>@sadbiwhore cara vc perdeu muito a oportunidade pois tinha na netflix ate umas semanas atras
+e drive com esse filme é uma raridade, so se vc quiser assistir com a qualidade de 4 pixels</t>
+  </si>
+  <si>
+    <t>quinta -feira cheio de trabalho,  tô  cansada, viu??
+estou em home office celestial...eu e a netflix!! o céu d verdade  é  na nossa casa, isso não  tem preço!!  ❤🙏 https://t.co/rzolvc1kff</t>
+  </si>
+  <si>
+    <t>elite way school, é você? https://t.co/5j9q6jxzbi</t>
+  </si>
+  <si>
+    <t>catálogo da netflix tá um lixo minha nossa</t>
+  </si>
+  <si>
+    <t>@netflixbrasil nossa eu amei? acho que vou assistir em netflix</t>
+  </si>
+  <si>
+    <t>as gravações de spencer chegaram ao fim! 
+sendo assim, qual dos projetos abaixo vocês acham que será o próximo a ser desenvolvido?
+▪️the chronology of water 
+▪️longa dirigido por ben foster
+▪️série 'a life in men' produzida por charlize theron (netflix) https://t.co/0zieztup4o</t>
+  </si>
+  <si>
+    <t>netflix eu te odeio, eu só queria assistir meu friends de novo</t>
+  </si>
+  <si>
+    <t>@_otakusbr netflix indo de mal a pior a cada dia. slk</t>
+  </si>
+  <si>
+    <t>na hora que a netflix finalmente me dá um cenário digno de fanfic na série #polosopostos
+eles são irmãos 
+aaaah não 🙄🙄</t>
+  </si>
+  <si>
+    <t>@lelerosam só a melhor produção da netflix</t>
+  </si>
+  <si>
+    <t>bruno já tem seu primeiro trabalho confirmado pela @netflixbrasil com gravações internacionais 😱👏🔥
+https://t.co/sfa4maf2av
+#brunogagliasso #ator #serie #netflix #santo #internacional #gravacoes #estreia #globo #atuação #famosos #tv #teledramaturgia</t>
+  </si>
+  <si>
+    <t>sobre relacionamentos 
+1. não 
+2. 3
+3. câncer 
+4. sim
+5. apegada 
+6. não 
+7. sim
+8. namorando
+9. jantar fora
+10. netflix em casa
+11. sim
+12. sim
+13. não 
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>aaaaaa vamboraaaaaaa
+netflix eu te amo https://t.co/m19pif5dvg</t>
+  </si>
+  <si>
+    <t>@eduardoleite_ @corsan_oficial até a chuva https://t.co/sl8hjsyktt</t>
+  </si>
+  <si>
+    <t>acabei de terminar de assistir na netflix o filme "mestres do yin-yang o sonho da eternidade" eu gostei bastante mais buguei muito com o plot twist, não que seja algo muito absurdo é que to meio lesado mesmo kkkkk</t>
+  </si>
+  <si>
+    <t>se a netflix não mostrar o gp da turquia eu serei obrigada a cometer um crime</t>
+  </si>
+  <si>
+    <t>@_animese @sifudemalucoo @ashhtalented é isso mesmo que eu li????? jojo na netflix??? agora todo mundo vai conhecer essa obra prima 👌🏻</t>
+  </si>
+  <si>
+    <t>ia ve um filme mas digitei neopets ao inves de netflix e so me toquei 20 min dps navegando no site sem rumo</t>
+  </si>
+  <si>
+    <t>fui assistir aquele filme da netflix, dia do sim, e agr tô com raiva daquelas crianças. bando de moleque mimado</t>
+  </si>
+  <si>
+    <t>1. não
+2. 1
+3. peixes
+4. não
+5. apegada
+6. nunca
+7. provavelmente ja fui
+8. solteira
+9. mandar flores  
+10. netflix em casa 
+11.  sim
+12. nn
+13. nn</t>
+  </si>
+  <si>
+    <t>@jpncunha1397 @arrascabigol1 @diegooliveiira_ @norton39 @futebol_info antes de começar o bbb já faturou 500 milhões, só uma marca para anunciar no bbb o valor eh 70 milhões, as assinaturas do globoplay passaram a netflix no brasil, chegou a 20 milhões, e as novelas faturam alguns milhões com breaks</t>
+  </si>
+  <si>
+    <t>@netflixbrasil apanha muito também ela né netflix kkk</t>
+  </si>
+  <si>
+    <t>eu estava sem nenhuma série pra assistir e achei na netflix e me interessei we love you kyndra https://t.co/b6cjfzzfko</t>
+  </si>
+  <si>
+    <t>@fraannnnnnnnn final de temporada nas séries da netflix</t>
   </si>
   <si>
     <t>@paulaaprad isso é um pouco triste na vdd, pq eu já quase zerei a netflix e não vi mais nada q me interessa e tb não sai temporada nova
 eu vou assistir o q dps? tô até com medo</t>
   </si>
   <si>
-    <t>@irismmonteiro os meus favs🙈🙈
-ação - my hero academia (heróis)
-attack on titan ( titãs e tal)
-terror - the promised neverland ( criança num orfanato e mais nao te digo)
-my hero tem na netflix, e os outros é so pesquisar no google</t>
-  </si>
-  <si>
-    <t>alguém avisa pro netflix que em “a sentinela” não existe soldada, todo dia eu entro na esperança de corrigirem mas talvez a militância seja mais forte que o português bem escrivido e dizido</t>
-  </si>
-  <si>
-    <t>a segunda temporada de b the beggining chegou na netflix!!!!!</t>
-  </si>
-  <si>
-    <t>queria estar assistindo filme de desenho na netflix fazendo massagem no pé dela</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. sim 
-2. 1
-3. leão 
-4. não 
-5. apegada 
-6. sim 
-7. sim 
-8. solteira
-9. jantar fora 
-10. netflix 
-11. sim 
-12. não sei 
-13. sim 
-curte que eu mando</t>
-  </si>
-  <si>
-    <t>@ssunduri quantos degrassi é que tem? é pq na netflix estou a ver degrassi: next class e só tem 4 temporadas</t>
-  </si>
-  <si>
-    <t>esse tempo só me faz pensar em netflix, cama, chocolate e não em aula de matemática pqp</t>
-  </si>
-  <si>
-    <t>e ai voces ja assistiram 'polos opostos' pra netflix não cancelar mais essa serie sobre patinação</t>
-  </si>
-  <si>
-    <t>1 hr rolando pela netflix e to quase assistindo diário de uma paixao de novo https://t.co/vxhoyygtng</t>
-  </si>
-  <si>
-    <t>@thorsouzaa aiii meu deussss feliz aniversárioooooo! muito sucesso e alegrias! saudades!!! 🥳🥳🥳🥳🥳🥰
-ps: te vejo na netflix</t>
-  </si>
-  <si>
-    <t>finalmente algo bom na netflix https://t.co/glywym0gcg</t>
-  </si>
-  <si>
-    <t>me indiquem séries pra mim assistir, q tenha na netflix</t>
-  </si>
-  <si>
-    <t>@joaopedrxfr kkkkkkkkkkkkkkkkkkkkkkkkkkkk vsfd bagulho ruim mano
-quando entrar na netflix eu vejo tudo mano prometo</t>
-  </si>
-  <si>
-    <t>eu avisei q depois do ova do rohan ia ter jojo na netflix e n e que vai ter mesmo. finalmente assistirei jojo na minha tv https://t.co/wpjx6iqakz</t>
-  </si>
-  <si>
-    <t>@whindersson trabalho freelancer 😊✍️
-empresas estão contratando várias pessoas para trabalhar como freelancer , como a netflix, facebook, instagram , entre outras!!!
-os ganhos são em média entre r$ 300 a r$ 600  por semana e r$ 1200 a r$ 2500 por mês...
-https://t.co/rvadaan1ge</t>
-  </si>
-  <si>
-    <t>esse final de semana vou ficar deboinha em casa e zerar a netflix</t>
-  </si>
-  <si>
-    <t>eu to maluco 🤪😜🤪😜🤪😜🤪😜 eu to na chuva 🌧️🌧️🌧️🌧️🌧️🌧️🌧️ eu to jojozado 🤪😜🤪😜🤪🤪😜 eu to jojozado ⚽⚽⏩🇧🇷🖤⏩🇧🇷🙅‍♂️⏩🇧🇷🙅‍♂️⏩🇧🇷 é jojo  porra🖤alo 📞📞📞📞 ai irmão 🗣️🗣️🗣️ é a tropa de jojo na netflix😎😎😎😎 vamoooooo eu to maluco 😜😜🤪😜🤪🤪 https://t.co/qldv7bx76i</t>
-  </si>
-  <si>
-    <t>enquanto na disney plus vc fica em dúvida qual foto de perfil colocar, na netflix vc tenta colocar o menos feio</t>
-  </si>
-  <si>
-    <t>você que gosta de anime e quer apreciar um anime bom e pequeno, a netflix botou kimetsu, aproveitem  e aprecie um bom anime</t>
-  </si>
-  <si>
-    <t>queria que a netflix só n tivesse divulgado o ator do wylan mas na real ele tá na série daí eu estaria assistindo e do nada “pah o wylan” seria muito emocionante mas sei que n passa de um sonho 😔</t>
-  </si>
-  <si>
-    <t>noah cameron schnapp é um ator norte-americano, mais conhecido por interpretar will byers na série de televisão stranger things da netflix e dar voz a charlie brown no filme the peanuts movie. está também em um novo filme chamado hubie halloween também da netflix.</t>
-  </si>
-  <si>
-    <t>jojo's bizarre adventure chegará a netflix em 8 de abril.
-especula-se de que o anime chegará ao serviço de streaming com dublagem local. https://t.co/mphbhayzi4</t>
-  </si>
-  <si>
-    <t>bruno gagliasso na netflix! o ator estará em santo, série espanhola criada por carlos lópez e com gravações no brasil e na espanha. no projeto, que conta ainda com o diretor vicente amorim e o roteirista gustavo lipsztein. bruno contracena com o ator espanhol raúl arévalo. https://t.co/zowwwbo6f5</t>
-  </si>
-  <si>
-    <t>vou ir assistir filme na netflix</t>
-  </si>
-  <si>
-    <t>e vamos de recesso simm,não tem outro jeito né hahah e bora maratonar as séries da disney e netflix 😌</t>
-  </si>
-  <si>
-    <t>netflix podia colocar uma opção para acelerar a velocidade do filme/série</t>
-  </si>
-  <si>
-    <t>era mentira moça eu não tenho netflix retire sua vestimenta https://t.co/utnj120gqf</t>
-  </si>
-  <si>
-    <t>em todos os filmes clichês e séries da netflix tem que haver alguém com aquele casaco jeans com pelinhos, sabe? sério, em todos</t>
-  </si>
-  <si>
-    <t>eu passo mal de rir com essas comparações. manu nunca ligou pra isso, não tá levantando um dedo pra ganhar seguidores e tá ocupada demais trabalhando e com o contrato milionário dela na netflix. acho que esquecem que quando a manu tava no bbb ganhava vários seguidores. https://t.co/vqspyxjflw</t>
-  </si>
-  <si>
-    <t>@octaviobuzz quando sair na feira ou na netflix eu vejo.</t>
-  </si>
-  <si>
-    <t>jojo vai vir pra netflix do brasil dia 8 de abril tomara que receba o reconhecimento que merece</t>
-  </si>
-  <si>
-    <t>tô sem netflix e tô doido pra termina de assistir the ranch</t>
-  </si>
-  <si>
-    <t>pro meus moots q nunca viram eu recomendo muito, tem na netflix e sim é um anime com muita sexualização, mas a maioria é tb né, fazer oq
-tem uma história muito legal por trás, mas tem uns temas pesados q são abordados do meio pro final</t>
-  </si>
-  <si>
-    <t>@bravu4u @shindoutakutoii @fantinha16 @popnerd38 pois deixaram disponível a dublagem na netflix americana, enquanto que aqui nem se pensava direito no anime ir pra netflix</t>
-  </si>
-  <si>
-    <t>a netflix tem seu começar a contratar ator de 16 anos pra interpretar personagens de 16 anos, não botar a porra de um menino de 23 anos pra interpretar um de 15</t>
-  </si>
-  <si>
-    <t>eu tava trsite e vi no catálogo da netflix e fui assistir we love you kyndra https://t.co/httkqqpgkt</t>
-  </si>
-  <si>
-    <t>eu tava andando pela netflix um dia antes de ser lançada na parte que tem os trailers e vi, e aí coloquei na minha lista pq achei legal
-https://t.co/cx7vtbgduv https://t.co/yifgwfzoi7</t>
-  </si>
-  <si>
-    <t>netflix anuncia série espanhola com bruno gagliasso  https://t.co/c1eydv6dit</t>
-  </si>
-  <si>
-    <t>tava pensando em dividir netflix com alguém, mas agora q vou ter aula, essa ideia seria mais um gatilho pra minha procrastinação</t>
-  </si>
-  <si>
-    <t>alguém me indica uma série da netflix pfvv</t>
-  </si>
-  <si>
-    <t>começando polos opostos... netflix se eu gostar dessa serie e vc cancelar mais uma série de patinação eu vou te abominar pra sempre</t>
-  </si>
-  <si>
-    <t>@foioguto algum dia vc vai fazer um video sobre gokushufudou? ele é um manga mas 8 de abril lança o anime na netflix</t>
-  </si>
-  <si>
-    <t>a netflix tá insuportável não tem nada pra ver</t>
-  </si>
-  <si>
-    <t>@figurante34 @op_netflix_fan @angelicaefrem nossa senhora, mas que arte perfeita</t>
-  </si>
-  <si>
-    <t>ter esse grande amor de clary e jace @kat_mcnamara @domsherwood1 perto de mim, é tudo o que me faz feliz #shadowhunters #saveshadowhunters #clace #jaceherondale #claryfairchild @constantinfilm @netflix @thecw https://t.co/h1qxg0zk1i</t>
-  </si>
-  <si>
-    <t>vocês têm ideia que essas fotos saiu ano passado? netflix por favor já chega!! estou morrendo de ansiedade https://t.co/laso0hmlac</t>
-  </si>
-  <si>
-    <t>@joooootape já tem outra série dele pra vir aí, ansioso pq única coisa de terror que presta na netflix é com ele</t>
-  </si>
-  <si>
-    <t>é que o lula rouba pra admirar a continha cheia só
-falar "nossa, olha quanto zero na conta" e pra poder pagar o netflix sem stress https://t.co/n0f34z9zls</t>
-  </si>
-  <si>
-    <t>@marrieterra amiga chama dawson’s creek tô vendo na netflix sério amiga vc vai surta kkkkkkk</t>
-  </si>
-  <si>
-    <t>mesmo com uma série muito hypada o disney+ não consegue bater em uma série da netflix por causa do dobro de assinantes https://t.co/czfrp89psu</t>
-  </si>
-  <si>
-    <t>@pbial hoje vai chamar a @majucoutinho para explicar o porquê o choro é livre, por favor, alguém me conte como foi... ficção eu prefiro a netflix
-@globonews @redeglobo @jornalbsm @tercalivre @taoquei1 @biakicis @carlazambelli38 @brasil_paralelo @brasilparalelo @jairbolsonaro</t>
-  </si>
-  <si>
-    <t>eu quase que faço unsubscribe à netflix quando carrego numa série para ver e aparece o “trailer” cheio de spoilers... q ódio https://t.co/zbea99ljod</t>
-  </si>
-  <si>
-    <t>@shinzoout https://t.co/7klohjlvwm
-se sua net aguenta uma netflix vai aguentar um torrent com seed razoável nisso aqui</t>
-  </si>
-  <si>
-    <t>era 10 horas da manhã eu tava vendo netflix
-do nada acordei as 15 hora sjkkkkjj</t>
-  </si>
-  <si>
-    <t>a produção mexicana mãe só tem duas conquistou o público e a netflix já confirmou uma segunda temporada.
-https://t.co/fjfgwcvudn</t>
-  </si>
-  <si>
-    <t>alguém pra me explicar tabula rasa da netflix ?</t>
-  </si>
-  <si>
-    <t>vi o trailer de sweet home da netflix e fiquei nervoso</t>
-  </si>
-  <si>
-    <t>o melhor ato da netflix 
-https://t.co/wuvr60u4b4</t>
-  </si>
-  <si>
-    <t>@caralhana one punch man eu tenho alguns mangás, mas não vi o anime no netflix, acho que vou assistir algum dia kkkkkkkkk</t>
-  </si>
-  <si>
-    <t>@ftozaa netflix carla diaz merece respeito</t>
-  </si>
-  <si>
-    <t>@wondershoi se um dia colocarem sailor moon clássico no catálogo da netflix vai ser necessário uma nova dublagem com remasterização vem aí...</t>
-  </si>
-  <si>
-    <t>esse títulos aleatórios da netflix é uma farsa 
-eu fico esperando algo realmente aleatório, e ela joga uma série que eu já assisto regularmente</t>
-  </si>
-  <si>
-    <t>que doideira tô até assustada, tava aqui procurando onde tinha sucker punch pq queria rever e esse filme n passa em canto algum aí dps de procurar no netflix, amazon prime e now, quando eu já tinha desistido...coloco na warner e o que tá dando? sucker punch amigos</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. n sei 
-2. 0 km novo de fabrica
-3. seila mermao
-4. nao sei
-5. apegado
-6. n tenho ex
-7. nao
-8. abandonado
-9. jantar fora
-10. netflix kakaka
-11. talvez
-12. sem expectativas 
-13. acho q sim
-curte que eu mando</t>
-  </si>
-  <si>
-    <t>eu to maluco 🤪😜🤪😜🤪😜🤪😜 eu to na chuva 🌧️🌧️🌧️🌧️🌧️🌧️🌧️ eu to jojozado 🤪😜🤪😜🤪🤪😜 eu to jojozado ⚽⚽⏩🇧🇷🖤⏩🇧🇷🙅‍♂️⏩🇧🇷🙅‍♂️⏩🇧🇷 é jojo  porra🖤alo 📞📞📞📞 ai irmão 🗣️🗣️🗣️ é a tropa de jojo na netflix😎😎😎😎 vamoooooo eu to maluco 😜😜🤪😜🤪🤪 https://t.co/7lqmmnqg4q</t>
-  </si>
-  <si>
-    <t>eu não acredito que "uma beleza fantástica" não ta mais na netflix, to muito triste</t>
-  </si>
-  <si>
-    <t>uma semana meus caros!
-restam 7 dias para a estreia de dota: dragon's blood no netflix.
-#dotadragonsblood https://t.co/rs5dzdnjla</t>
-  </si>
-  <si>
-    <t>netflix vai produzir serie de tomb raider e cowboy bebop putzz caras o empenho dessa empresa em destruir a memoria afetiva das pessoas</t>
-  </si>
-  <si>
-    <t>@thaisespos @netflixbrasil @esposbrasil tem que divulgar no ig tbm pro alcance ser maior @netflixbrasil 
-por favor netflix nunca te pedi nada 😭</t>
-  </si>
-  <si>
-    <t>desde que acabei a última temp de como defender um assassino eu abandonei o netflix preciso de uma série boaaaa</t>
+    <t>nunca vou entender a netflix ter cancelado spin out e um ano depois ter lançado outra série de patinação onde a protagonista parece muito kaya scodelario (em spin out) em certos momentos, tem hora que eu acho que to assistindo a mesma série (????????)</t>
+  </si>
+  <si>
+    <t>netflix tirou todas as mnhs séries preferidas, qq vou assistir nessa merda agr ?</t>
+  </si>
+  <si>
+    <t>comecei o novo anime da netflix
+o snipermask é mt lindo meudeus do céu me come de ladinho https://t.co/du55a68g5d</t>
+  </si>
+  <si>
+    <t>@weekndpink tô vendo o corte normal na netflix, mas já tem drive pelo tt do snyder cut vou assistir por drive https://t.co/92boyk6dtb</t>
+  </si>
+  <si>
+    <t>minha saudade tem nome, sobrenome, elenco, ótima atuação e um casal com química. a verdade é que spin out tinha tudo para ser um sucesso com várias temporadas. é uma pena que a netflix não tenha entendido essa obra de arte. https://t.co/copx6odnsx</t>
+  </si>
+  <si>
+    <t>minha vida começou a desandar quando friends saiu da netflix</t>
+  </si>
+  <si>
+    <t>@doougfuny to na expectativa ja e amanhã ainda sai tbm aquela da formula 1 na netflix. bastante coisa pra maratonar. hahahaha
+ah e o snyder cut nem animei, 4h é muito num filme. hahahahah</t>
+  </si>
+  <si>
+    <t>vamos pq se depender da netflix... sky rojo tomorrow</t>
+  </si>
+  <si>
+    <t>e eu reclamando do selo da netflix na edição br. desculpa https://t.co/wkqekcjl9d</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa que acima da alina só o helicóptero da polícia</t>
+  </si>
+  <si>
+    <t>torrent disney e netflix salvando minha vida nesses últimos tempos https://t.co/qfoifwq7ur</t>
+  </si>
+  <si>
+    <t>é crime só ter 4 temporadas viu netflix sua puta piranha vadia @netflixbrasil</t>
+  </si>
+  <si>
+    <t>@manuriosnotice @jsantos455 tá todo mundo pedindo o hot deles @netflix</t>
+  </si>
+  <si>
+    <t>@lacastelleone_ a risque faz o papel dela enquanto netflix só decepciona</t>
+  </si>
+  <si>
+    <t>serviço bom é o meu, não faz nada o dia inteiro com direito a netflix</t>
+  </si>
+  <si>
+    <t>@mariane76278983 pq perdeu tempo otaria? eu teria assistido netflix kkkkk tu e otaria msm ne? kkkkkk</t>
+  </si>
+  <si>
+    <t>se estar e netflix com pizza ou uma boa resenha com os amigos  passou a ser o melhor programa da vida ultimamente né ?! 
+a gente tá ficando velho gente ☹️😞</t>
   </si>
   <si>
     <t>sobre relacionamentos 
@@ -1684,167 +1170,672 @@
 curte que eu mando</t>
   </si>
   <si>
+    <t>acabei de ver aqui que o filme o senhor estagiário com robert deniro vai sair do ar na netflix dia 31 de março, assistam gente! é muito inspirador</t>
+  </si>
+  <si>
+    <t>@maxpettersonm isso é o prédio da netflix?</t>
+  </si>
+  <si>
+    <t>@twolana9 netflix 
+forças complex</t>
+  </si>
+  <si>
+    <t>tá eu e minha sogra assistindo filme na netflix</t>
+  </si>
+  <si>
+    <t>esse filme com a kristin davis q estreou na netflix deadly illusions é bonzinho até, uma junção de mulher solteira procura com a mão que balança o berço 🤪</t>
+  </si>
+  <si>
+    <t>diamond is unbreakable chegando na netflix. jojo dublado já é realidade.</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix e a segunda temporada de unité 42? 😭😭</t>
+  </si>
+  <si>
+    <t>#tbt para esse dia icônico que louis hofmann (jonas, de dark) falou sobre “estar de volta filmando a s2 de the rain” e lucas repostou “obrigado ao meu dublê de cenas difíceis. não conseguiria sem você” 
+uma colaboração, hein netflix! 👀 
+📸 louishofmann https://t.co/jp0apzx9lk</t>
+  </si>
+  <si>
+    <t>@yamietchelouz se re contra festeja con vino blanco mirando netflix</t>
+  </si>
+  <si>
+    <t>quem quiser indicar série que tenha na netflix,eu to aceitando ta :)</t>
+  </si>
+  <si>
+    <t>@harlancoben @stayclosehc @realmikefox @murderbooks estou assistindo safe on netflix 👏🏼👏🏼👏🏼série maravilhosa.. @harlancoben um grande escritor!!!</t>
+  </si>
+  <si>
+    <t>@_duarterodrigo hoje lança drive to survive 3 no netflix, mais um motivo hahhahaha</t>
+  </si>
+  <si>
+    <t>netflix é um bom site só ficaria melhor com as novas temporadas de gumball</t>
+  </si>
+  <si>
+    <t>@isaftany estamos achando que ele vai trabalhar com o bruno gagliasso na netflix</t>
+  </si>
+  <si>
+    <t>acabei de assistir o filme "por trás da inocência" da netflix. me interessou por ninguém estar entendendo o filme, e eu entendi ele perfeitamente. será que sou doida? 😂</t>
+  </si>
+  <si>
+    <t>quero trocar a foto da netflix mas a jennie é tão linda q fico com dó de tirar 😭</t>
+  </si>
+  <si>
+    <t>@cgklebao quer ver a carinha linda dele? vá ver as produções da netflix.</t>
+  </si>
+  <si>
+    <t>queria mto ver vicenzo até ia chamar el* para ver tbm... so q fui olhar e é original netflix ai vc fode ne</t>
+  </si>
+  <si>
+    <t>@davidwe32380311 @fabiorrluz74 @portugassis verdade pois fate tem um público mais nicho, kimetsu vai vir dublado em pt br em abril na netflix aí talvez mais pessoas conheçam e o manda vende pra caraí.</t>
+  </si>
+  <si>
+    <t>nem pra marvel olhar para os oprimidos e colocar a série do loki na netflix e não no disney+😔😔</t>
+  </si>
+  <si>
+    <t>acho que vou trocar a netflix pelo disney+ !</t>
+  </si>
+  <si>
+    <t>tava lá na netflix naquela aba de lançamento daí achei lá gostei da sinopse e assisti 
+we love you kyndra https://t.co/2s2nmoknjy</t>
+  </si>
+  <si>
+    <t>que netflix oque
+que transar oque
+vem aqui em casa pra gente maratonar over the garden wall 😍😍😍🥰🥰🥰😎😎😎🤠🤠🥺🤧</t>
+  </si>
+  <si>
+    <t>não acho uma série boa na netflix, prime vídeo, globo play e disney+</t>
+  </si>
+  <si>
+    <t>a conjuradora do sol chegou!! ☀️☀️ sombra e ossos estreia dia 23 de abril na netflix, será que vem trailer logo?  https://t.co/4wmd6c4yox</t>
+  </si>
+  <si>
+    <t>@netflixbrasil a cara de felicidade da alina meu deus netflix vou chorar</t>
+  </si>
+  <si>
+    <t>netflix vai tirar o shrek do catálogo, minha filha vai enlouquecer ela assiste todo dia</t>
+  </si>
+  <si>
+    <t>@perobensee eu acho muito bom pq por mais que sejam "filmes interativos" eles não funcionariam bem fora do video game, não teria a mesma fluidez e imersão (basta ver bandersnatch ou qualquer coisa interativa da netflix e comparar com what remains of edith finch por exemplo)</t>
+  </si>
+  <si>
+    <t>alguem sabe de algum app que da pra ver series de graça que ainda nao foram lançados na netflix ou que ja sairam do ar</t>
+  </si>
+  <si>
+    <t>sério perdi td isso eh roteiro de série da netflix</t>
+  </si>
+  <si>
+    <t>descobri q tem na netflix, esse eh o motivo do meu colapso https://t.co/e3p31mvact</t>
+  </si>
+  <si>
+    <t>pelo o que eu acompanho o lewis ele parece ser uma pessoa que gosta de ficar calmo e não gosta que ficam em cima dele, pq ele ia querer uma equipe de filmagem da netflix em cima dele durante um gp??? se ele não aparecer no dts é pq ele não quer, não é pq ele tá sendo ignorado</t>
+  </si>
+  <si>
+    <t>vou ir assistir filme na netflix</t>
+  </si>
+  <si>
+    <t>não aguento mais minha netflix sendo hackeada</t>
+  </si>
+  <si>
+    <t>fui ver o filme novo da netflix e só confirmei que eu realmente não gosto de criança pqp</t>
+  </si>
+  <si>
+    <t>@arakisbasement cara, dependendo do tanto de gente na sala do zoom eu acho q daria, na minha sala da escola tinha 100 pessoas na mesma sala ao mesmo tempo no zoom, mas o problema de direito autoral é meio complicado mesmo, mas se servir de consolo jojo tá chegando na netflix no brasil+</t>
+  </si>
+  <si>
+    <t>era 10 horas da manhã eu tava vendo netflix
+do nada acordei as 15 hora sjkkkkjj</t>
+  </si>
+  <si>
+    <t>@marbundas a mulher não da ponto sem nó amigo 🗣🗣🗣 e a lenda ainda tá riquíssima agora empregada pela netflix</t>
+  </si>
+  <si>
+    <t>@gabiu_twt eu tenho certeza que ela teria tido um revival na carreira numa série da netflix</t>
+  </si>
+  <si>
+    <t>eu não estou assistindo todas as séries q eu já assisti td dnv só pq não tem mais oque eu assistir nessa netflix e não tem nd pra eu fazer da vida</t>
+  </si>
+  <si>
+    <t>o homem do futuro (2011)
+dir.: cláudio torres
+disponível na netflix https://t.co/bsqae38ych</t>
+  </si>
+  <si>
+    <t>isso ou aquilo
+dia x noite
+futebol x vôlei 
+cinema x netflix
+frio x calor
+doce x salgado
+inverno x verão
+outono x primavera
+bbb x a fazenda 
+praia x piscina 
+rbd x rbr
+lua x sol
+cidade x campo
+filme x série
+ comédia x terror
+responda com a tag forças complex</t>
+  </si>
+  <si>
+    <t>@anapaulavolei com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>@hessaflame amgg eu amava, até que um dia minha conta na netflix bugou e não sei onde parei, ai não terminei</t>
+  </si>
+  <si>
+    <t>saudades assistir t70s e full house na hora do almoço mas a netflix tinha que tirar elas do catálogo né 😔</t>
+  </si>
+  <si>
+    <t>@nalaurachiq tem um na netflix de uma assassina, não lembro se tem festa, mas tem vestido chique ava o nome</t>
+  </si>
+  <si>
+    <t>queria uma tarde nublada com chuva, netflix e pipoca 
+lembrei que tenho que estudar 🤡</t>
+  </si>
+  <si>
+    <t>@saugaudinho_ em casa vc pode aumento dar um alt tab no netflix</t>
+  </si>
+  <si>
+    <t>eu nunca vo perdoar a netflix por cancelar i am not okay with this 😭😭 q odio</t>
+  </si>
+  <si>
+    <t>estou sem netflix fml meu mundo desmoronou😭</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estrelará série espanhola de ação da netflix https://t.co/clfjmiay0h https://t.co/gqfbffmvb2</t>
+  </si>
+  <si>
+    <t>@netflixbrasil eu to ansiosa aqui netflix me ajuda não aguento esperar</t>
+  </si>
+  <si>
+    <t>pro pessoal que polariza as eleições 2022 entre lula e bolsonaro, indico ver (ou rever):
+o mecanismo (netflix) 
+a lei é para todos 
+retrato narrado (spotify) 
+pra refrescar a memória e ver que nenhum deles merece chegar ao segundo turno, caso se candidatem.</t>
+  </si>
+  <si>
+    <t>seja hamilton, max, seb, ricciardo, wtv... é horrível a netflix não mostrar o momento em que um piloto se torna campeão do mundo. alias, não fazer 1 episódio dedicado a esse tema é absurdo. neste caso particular, ainda pior com um piloto q igualou um record histórico de 7 titulos https://t.co/yz3jreiui1</t>
+  </si>
+  <si>
+    <t>eu não lembro direito, eu acho que vi alguém na tml falando e dps apareceu no catálogo da netflix pra mim 
+we love you kyndra https://t.co/5w5z1biu9j</t>
+  </si>
+  <si>
+    <t>@fb_lewandowski se a netflix não cancelar pelo cronograma a segunda temporada só em 2022😥😥😥😥</t>
+  </si>
+  <si>
+    <t>eu: “you” é a pior série da netflix, sem condições
+eu tbm: vou ver só mais um episódio</t>
+  </si>
+  <si>
+    <t>netflix tá perdendo essa guria como roteirista</t>
+  </si>
+  <si>
+    <t>@l_ramos14 ta mas ei tenho a netflix do japão https://t.co/hpwnenhgxa</t>
+  </si>
+  <si>
+    <t>series de adolescente na netflix são assim https://t.co/sdpegldvvx</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix avisa que ninguem esta acima de alina starkov 🗣🗣🗣🗣</t>
+  </si>
+  <si>
+    <t>ligar tv agora só pra assistir netflix, tô ficando com mais pânico com as notícias do covid! 😢😓😓</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix me fala uma série boa</t>
+  </si>
+  <si>
+    <t>@netflixbrasil @ravkabr netflix sua p cade o conteúdo helnik</t>
+  </si>
+  <si>
+    <t>@cryforkenma por favor vamo ver juntinhas quando tiver na netflix 😭😭😭😭😭</t>
+  </si>
+  <si>
+    <t>@cshimada hahaha brigado lindissimaa❤️ olha se depender das materias q eu to tendo tem um processo longo até a netflix hahahah mas fé</t>
+  </si>
+  <si>
+    <t>sobre relacionamentos 
+1. não 
+2. 2
+3. não sei?????
+4. não 
+5. apegada
+6. depende de qual
+7. sim
+8. solteira
+9. jantar
+10. netflix
+11. sim
+12. acho que não 
+13. essa eu deixo no ar
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>queria mais séries norueguesas na netflix, amo aquele país, é tão lindo 😢</t>
+  </si>
+  <si>
+    <t>sobre relacionamentos 
+1.não 
+2. 2
+3. peixes 
+4.tô em um
+5.apegada
+6.não 
+7. não 
+8.namorando
+9.janta fora
+10. netflix em casa
+11. não 
+12. tá cringe 🥲
+13. não 
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>@seenyoucry então, demora uns episódios pra gostar pq eles dão uma enrolada, mas achei um anime bom até kakaka
+tem a primeira temporada na netflix e os episódios são bem curtinhos</t>
+  </si>
+  <si>
+    <t>@coralinekkk sim já aconteceu cmg, inclusive, tem um filme na netflix chamado koe no katachi q uma mina surda sofre bullying dps ficam super amgs lá e tals</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix eu vou ter um surto meu deus é ela caras</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estreia 'santo', produção internacional da netflix
+categorizado como thriller policial, o roteiro de miguel ángel fernández e gustavo lipsztein flerta com o terror @netflixbrasil @brunogagliasso 
+https://t.co/vxhklgtxg1 https://t.co/ddpf3cd1he</t>
+  </si>
+  <si>
+    <t>meu deus eu vi agora que tem voltron na netflix https://t.co/nmlp37b2cx</t>
+  </si>
+  <si>
+    <t>tempinho bom pra ficar vendo netflix deitada com mozao</t>
+  </si>
+  <si>
+    <t>eu fui ver minha lista da netflix e so tem dorama e anime</t>
+  </si>
+  <si>
+    <t>saiu a decima primeira temporada de modern family na netflix ovo chora</t>
+  </si>
+  <si>
+    <t>os 7 pecados capitais estão no mundo digital. 
+preguiça - netflix
+luxúria - tinder
+vaidade - instagram 
+ira - twitter 
+inveja - facebook 
+gula - ifood 
+soberba - linkedin</t>
+  </si>
+  <si>
+    <t>ia ver uma série ai netflix bugou e apareceu outra baseada em crimes reais e agora vo assistir essa outra</t>
+  </si>
+  <si>
+    <t>velozes e furiosos vai sair do catalogo da netflix, declaro aqui a minha tristeza e indignação</t>
+  </si>
+  <si>
+    <t>#cinema | indicado ao oscar, curta palestino entra no cardápio da netflix - https://t.co/tdbiwyvsgy https://t.co/ckdnakaqxs</t>
+  </si>
+  <si>
+    <t>quando paro p almoçar viajo no netflix! é meu momentinho de ver serie ou filme ai mt bom, amo almoçar sozinha</t>
+  </si>
+  <si>
+    <t>@netflixbrasil ela precisa ser a américa de a seleção. tá ouvindo netflix????</t>
+  </si>
+  <si>
+    <t>eu tava andando pela netflix um dia antes de ser lançada na parte que tem os trailers e vi, e aí coloquei na minha lista pq achei legal
+https://t.co/cx7vtbgduv https://t.co/yifgwfzoi7</t>
+  </si>
+  <si>
+    <t>@czndyk tem no netflix essa que eu to vendo</t>
+  </si>
+  <si>
+    <t>climinha bom para estar deitada olhando uma netflix</t>
+  </si>
+  <si>
     <t>@xunqievil vamo espera entra na netflix p gent ver amor entra mês que vem</t>
   </si>
   <si>
-    <t>@gincanafriend avisa que é a série melhor da netflix</t>
-  </si>
-  <si>
-    <t>impressionante como a netflix caga em um todos finais que faz, o recepcionista é um baita filma, mas o final é cagado</t>
-  </si>
-  <si>
-    <t>@netflixbrasil netflix o filme de a seleção ta aí né imagina ela sendo rainha como america singer? amo?!</t>
-  </si>
-  <si>
-    <t>@alicesaquino oi, fala sobre polos oposto (série nova da netflix) :)</t>
-  </si>
-  <si>
-    <t>essa temporada da fazenda deveria estar na netflix https://t.co/fnkonen3hi</t>
-  </si>
-  <si>
-    <t>meu deus eu criei um romance de netflix desisti de medicina vou virar escritor fodas @netflixbrasil se estiver interessada manda uma dm</t>
-  </si>
-  <si>
-    <t>vai ter que ir todo mundo fazer barraco no perfil da netflix é???</t>
-  </si>
-  <si>
-    <t>quando teremos um documentário do bts na netflix pra eu poder usar icon do yoongi</t>
+    <t>fui ver o primeiro episódio de tiger &amp;amp; bunny na netflix e... q triste, eles tiraram as propagandas
+na versão original todos os uniformes dos heróis tinham propagandas do mundo real, era uma crítica (q ao mesmo tempo se vendia) e era super engraçado também https://t.co/obboejdllz</t>
+  </si>
+  <si>
+    <t>@_animese jojo na netflix talvez dublado 
+kimetsu na netflix dublado 
+tp 2 de kimetsu  
+filme de kimetsu
+2 eventos grabdes de jojo onde provavelmente vao anunciar a parte 6
+klr minha sorte virou do nada</t>
+  </si>
+  <si>
+    <t>caio criou uma conta infantil pra mim na netflix kkkkkkk</t>
+  </si>
+  <si>
+    <t>@imirnac eu ai quando tinha netflix</t>
+  </si>
+  <si>
+    <t>fui toda tonta abrir netflix pra assistir sociedade dos poetas mortos e confirmar que o menino lá realmente parece o gansey 
+e vejo que a netflix tirou 🤡🤡🤡🤡 
+mais uma derrota pra trc stan</t>
+  </si>
+  <si>
+    <t>algum dos filmes concorrendo ao oscar, de modo geral, está no netflix ou no amazon prime? 
+eu vou ver a maioria, de qualquer modo, só estou querendo saber quais já posso ir facilitando por aqui pra encontrar.</t>
+  </si>
+  <si>
+    <t>@rafaeld55315425 acho que kimetsu vai ser o primeiro filme de anime ( se passar no cinema) que eu vou chorar e ficar mais feliz de estar vendo no cinema , nem dragon ball me deixou tão empolgado assim, o bom é que ele já vai entrar no hype, pois dia 1 de abril estreia dublado na netflix+</t>
+  </si>
+  <si>
+    <t>@joooootape já tem outra série dele pra vir aí, ansioso pq única coisa de terror que presta na netflix é com ele</t>
+  </si>
+  <si>
+    <t>@nikofscars adoro que já apareceram os 5 menos o meu filho
+a netflix é wylanfobica so pode</t>
+  </si>
+  <si>
+    <t>fácil chegar nos 14 milhões quero ver ela sair do bbb e a netflix querer assinar contratinho</t>
+  </si>
+  <si>
+    <t>@netflixbrasil a maior do mundo netflix! só fica escuro quando ela diz que fica!</t>
+  </si>
+  <si>
+    <t>kayky falou q meu quarto tá q nem hotel, c televisão c netflix , ar ventidor, cama, som kkk</t>
+  </si>
+  <si>
+    <t>e ai voces ja assistiram 'polos opostos' pra netflix não cancelar mais essa serie sobre patinação</t>
+  </si>
+  <si>
+    <t>fiquei apaixonada em the one, netflix q n ouse cancelar essa série perfeita</t>
+  </si>
+  <si>
+    <t>pessoas, vídeo novo!
+no vídeo de hoje vou comentar sobre o anúncio de jojo no catálogo da netflix e sobre a possível dublagem do anime.
+espero que gostem, link nos comentários! https://t.co/nrub4kwsci</t>
+  </si>
+  <si>
+    <t>só queria ta de boa vendo um netflix cm a gata mas falto a gata...</t>
+  </si>
+  <si>
+    <t>se a netflix colocar jojo começando pela parte 3 eu explodo aquela empresa</t>
+  </si>
+  <si>
+    <t>@stf_oficial quem vai me obrigar ir no cinema assistir porcaria, baixei alguns no netflix não gostei, deletei, procuro selecionar, não é qualquer porcaria que assisto, simples assim, para de interferir em nossas escolhas. prisão em 2ª instância é mais importante para ficarmos livre do lula.</t>
+  </si>
+  <si>
+    <t>@bravu4u @shindoutakutoii @fantinha16 @popnerd38 pois deixaram disponível a dublagem na netflix americana, enquanto que aqui nem se pensava direito no anime ir pra netflix</t>
+  </si>
+  <si>
+    <t>essa série que a netflix lançou polos opostos é tão ruim meu deus perdi meu tempo</t>
+  </si>
+  <si>
+    <t>é que o lula rouba pra admirar a continha cheia só
+falar "nossa, olha quanto zero na conta" e pra poder pagar o netflix sem stress https://t.co/n0f34z9zls</t>
+  </si>
+  <si>
+    <t>sobre relacionamentos 
+1. não 
+2. 5
+3. sagitário 
+4. não 
+5. apegada
+6. claro kakakakmm
+7. sim
+8. solteira
+9. flores
+10. netflix 
+11. sim
+12. nunca se sabe
+13. não 
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>@vkpalet fez isso, inclusive ele &amp;gt;inyeop&amp;lt; recebeu bastante atenção da mídia, e do público e etc até brincaram que ele era o novo 30 but 17 de la. rolou uma especulação sobre o papel dele em um drama que a netflix vai produzir mas nunca confirmaram realmente</t>
+  </si>
+  <si>
+    <t>"se algo acontecer... te amo." ficou conhecido por arrancar lágrimas com seu roteiro emocionante sobre luto. você pode vê-lo na netflix https://t.co/qni1kl7tcf</t>
+  </si>
+  <si>
+    <t>nao consigo tirar print da netflix, q cu</t>
+  </si>
+  <si>
+    <t>1.não
+2.nenhuma
+3.libra
+4.depende da pessoa
+5.apegado
+6.depende
+7.não 
+8.solteiro
+9.jantar fora 
+10. netflix em casa
+11.acho que sim
+12.não sei como vai ser esse ano 
+13.acho que não,nao sei 
+curte que eu mando</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix me dá a data da 5b de lucifer e eu digo se esperava ou não</t>
+  </si>
+  <si>
+    <t>e agora como posso assistir gossip girl pela oitava vez se a netflix tirou do catálogo</t>
+  </si>
+  <si>
+    <t>gente a netflix lançou um doc sobre a educação americana: fraude e privilégio.
+que documentário chocante... se assemelha um pouco ao que acontece nas universidades federais daqui.</t>
+  </si>
+  <si>
+    <t>pro meus moots q nunca viram eu recomendo muito, tem na netflix e sim é um anime com muita sexualização, mas a maioria é tb né, fazer oq
+tem uma história muito legal por trás, mas tem uns temas pesados q são abordados do meio pro final</t>
+  </si>
+  <si>
+    <t>@hydrilmoon @shadowandbone_ @gabsmeu a cada teaser q sai eu calculo o número de séries q a netflix teve q cancelar só pros efeitos de shadow and bone</t>
+  </si>
+  <si>
+    <t>se minha mãe é uma peça ganhasse uma adaptação coreana o título em inglês na netflix seria my mother is playful</t>
+  </si>
+  <si>
+    <t>#economia | lucro da caixa em 2020 chega a r$ 13,169 bilhões, com queda de 37,5% - https://t.co/8iycmb6j44 https://t.co/eambn0hbdt</t>
+  </si>
+  <si>
+    <t>se fosse por dificuldade, ainda assim não justifica mas por pura futilidade, netflix, uber, amazon aaaa vtnc</t>
+  </si>
+  <si>
+    <t>@netflixbrasil linda amo ela netflix avisa que ela é abpatroa vade o nikolai</t>
+  </si>
+  <si>
+    <t>@andregostoso14 @animeinjapann eu vi só o primeiro episódio, mas tem a abertura no youtube no canal da netflix, mas é oq vc disse fez sentido.</t>
+  </si>
+  <si>
+    <t>bruno gagliasso estreia em santo, série original espanhola da netflix https://t.co/emdtdi2r8t</t>
+  </si>
+  <si>
+    <t>ter esse grande amor de clary e jace @kat_mcnamara @domsherwood1 perto de mim, é tudo o que me faz feliz #shadowhunters #saveshadowhunters #clace #jaceherondale #claryfairchild @constantinfilm @netflix @thecw https://t.co/h1qxg0zk1i</t>
+  </si>
+  <si>
+    <t>tava olhando uma série na netflix e aí ela achou 💔 e como é de patinação no gelo provavelmente será cancelada</t>
+  </si>
+  <si>
+    <t>galera, segunda temporada de love alarm 
+como eu n lembro nada da primeira kkkkk torci p hye-yeong
+mas serio, foi muito parada, exploraram pouquissimo os personagens, senti sono 75% do tempo
+to decepcionada, dona netflix.
+atores bons
+primeira temporada boa
+tinha a faca e o queijo</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix lenda eu sempre te amei</t>
+  </si>
+  <si>
+    <t>sim conseguiu ser melhor com jojo na netflix aaaaa</t>
+  </si>
+  <si>
+    <t>11 
+tava com tempo livre e decidi caçar algo pra ver na netflix https://t.co/wmtxh1szqc https://t.co/aa6mimjez0</t>
+  </si>
+  <si>
+    <t>eu tô triste de verdade com a retirada de merlí da netflix. não entra na minha cabeça como podem tirar uma série tão foda, necessária e rica em conhecimento que eles mesmos produziram 😭</t>
+  </si>
+  <si>
+    <t>a série do patrão família dia 23/04 na netflix 🥺💕🎩 https://t.co/1yxwqiipeq</t>
+  </si>
+  <si>
+    <t>crl que odio q eu tenho da netflix q n diz o lugar certo que eu parei na desgraça da serie q odioooooooooo</t>
+  </si>
+  <si>
+    <t>@jornalbsm com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>comédia policial à brasileira, cabras da peste estreia na netflix. veja mais em: tribuna do sertão - https://t.co/d2amgr9gwb</t>
+  </si>
+  <si>
+    <t>e vamos de recesso simm,não tem outro jeito né hahah e bora maratonar as séries da disney e netflix 😌</t>
+  </si>
+  <si>
+    <t>@fabriciocarlet1 acho que a força da marca disney pesa muito. mas o produto em si é fraco. 
+catálogo muito reduzido. assinei 2 meses e cancelei. nem a minha filha tava gostando, salvo um ou outro filme. netflix e prime vídeo eu mantenho.</t>
+  </si>
+  <si>
+    <t>enquanto na disney plus vc fica em dúvida qual foto de perfil colocar, na netflix vc tenta colocar o menos feio</t>
+  </si>
+  <si>
+    <t>e eu descobri so agora que o titus de unbreakanle kimmy shmidt  apresenta esse vem cantar na netflix como eu amo este gay meodeus</t>
+  </si>
+  <si>
+    <t>trabalhando,estudando,lendo e assistindo netflix.
+estou me sentindo minha mãe</t>
+  </si>
+  <si>
+    <t>eu não tenho netflix para assistir sky rojo. pobre não tem um dia de paz</t>
+  </si>
+  <si>
+    <t>merda de netflix que não tem nanatsu no catálogo</t>
+  </si>
+  <si>
+    <t>@jtbageston ela veio assistir netflix msm sabendo q n tinha</t>
   </si>
   <si>
     <t>@diogomainardi @pbial hoje vai chamar a @majucoutinho para explicar o porquê o choro é livre, por favor, alguém me conte como foi... ficção eu prefiro a netflix
 @globonews @redeglobo @jornalbsm @tercalivre @taoquei1 @biakicis @carlazambelli38 @brasil_paralelo @brasilparalelo @jairbolsonaro</t>
   </si>
   <si>
-    <t>as vezes eu tô de boa e lembro da presepada que a netflix fez com os fãs quando resolveu produzir aquela 2 temporada ridícula do love alarm</t>
-  </si>
-  <si>
-    <t>preciso ter você @kat_mcnamara sempre junto do meu coração #shadowhunters #saveshadowhunters #claryfairchild @constantinfilm @netflix @thecw https://t.co/cjemf2bqao</t>
-  </si>
-  <si>
-    <t>netflix eu te odeio por estragar os prints das cenas</t>
-  </si>
-  <si>
-    <t>@angelicaefrem @op_netflix_fan @missbushiido eu tô sonhando com esse hiluluk no live action no meio da aula, e já tô lembrando dele 
-oda seu monstro tá me fazendo ter depressão na hora da aula</t>
-  </si>
-  <si>
-    <t>diamond is unbreakable chegando na netflix. jojo dublado já é realidade.</t>
+    <t>uma semana meus caros!
+restam 7 dias para a estreia de dota: dragon's blood no netflix.
+#dotadragonsblood https://t.co/rs5dzdnjla</t>
+  </si>
+  <si>
+    <t>queria que o otis assistisse jojo agora que vai sair na netflix, ia ser mais fácil....</t>
+  </si>
+  <si>
+    <t>o melhor ato da netflix 
+https://t.co/wuvr60u4b4</t>
+  </si>
+  <si>
+    <t>meu professor de direito internacional pegou pesadíssimo em mandar fazermos uma resenha crítica comparando o caso do chile que foi condenado por censurar um filme que envolvia a fé cristã vs. o caso do especial de natal do porta dos fundos que foi retirado da netflix...</t>
+  </si>
+  <si>
+    <t>@netflixbrasil mil anos depois, né, dona netflix??</t>
+  </si>
+  <si>
+    <t>@badgallayss tinha na netflix tbm, mas eu odeio a dublagem de lá, é isso amg! https://t.co/ktr0kta1ze</t>
+  </si>
+  <si>
+    <t>eu acho q deu pau na minha netflix https://t.co/x0qj8enwhf</t>
+  </si>
+  <si>
+    <t>#meupaieoutrosvexames estreia na netflix em 14 de abril de 2021.
+https://t.co/000so357vc</t>
+  </si>
+  <si>
+    <t>@netflixbrasil devo estudar ou assistir netflix?</t>
+  </si>
+  <si>
+    <t>pela aba de em breve da netflix (ficou na minha lista por tipo um mês e dps comecei a ver fotos no instagram delas e comecei a assistir)
+we love you kyndra https://t.co/wqqqf3jo2l</t>
+  </si>
+  <si>
+    <t>ansiosa desde já https://t.co/s8atkposqf</t>
+  </si>
+  <si>
+    <t>ai você passa um tempão assistindo 36 episódios de uma série, #colony na @netflix para só agora saber que ela não terá prorrogação e jamais terá um final da história. me sinto enganado @netflixbrasil</t>
+  </si>
+  <si>
+    <t>eu saindo 6h da manhã e voltando 21h da noite, minha mãe:
+[18/3 14:50] mãe: tou assistindo filme  na tua netflix
+[18/3 14:50] mãe: no meu celular kkkkk
+kkkkkkkkkkkkk amo</t>
+  </si>
+  <si>
+    <t>@radardamidia @jairbolsonaro com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>imagens chocantes:
+veja como está o tom holland após ser demitido pela marvel e pela netflix. https://t.co/dz7l1skrn0</t>
+  </si>
+  <si>
+    <t>@zzizzarv @shaygrudolph é a atriz que fez a dawn na 1° temporada da série baby sitters club da netflix e agora ela faz a america chavez na marvel (inclusive vai estar no novo filme do doutor estranho)</t>
+  </si>
+  <si>
+    <t>tá tudo uma merda= vou assistir netflix</t>
+  </si>
+  <si>
+    <t>@ssunduri quantos degrassi é que tem? é pq na netflix estou a ver degrassi: next class e só tem 4 temporadas</t>
+  </si>
+  <si>
+    <t>@zouishabit91s acho que não 
+tem na netflix/disney+?</t>
+  </si>
+  <si>
+    <t>2021 e eu ainda não superei que a netflix cancelou the society</t>
+  </si>
+  <si>
+    <t>@netflixbrasil netflix para de fazer série e foca apenas em s&amp;amp;b quero tudo perfeito nessa série</t>
+  </si>
+  <si>
+    <t>@pevensievans acorda best,daqui a pouco a netflix lança a braba</t>
+  </si>
+  <si>
+    <t>@hatesannal vai entrar na netflix agr vc vai assistir comigo ou nao putinha 🙈 https://t.co/0wusg3kusv</t>
+  </si>
+  <si>
+    <t>@25o8s que demora agiliza netflix eu preciso ve com minha namorada</t>
+  </si>
+  <si>
+    <t>@hanieely olhando aqui na netflix lembrei que tenho orphan black para terminar também,, ja deve fazer uns 4 anos kkkkkkkkkkkkkkkk se eu procurar deve ter mais</t>
+  </si>
+  <si>
+    <t>@dimacgarcia com geladeira cheia, conta no banco positiva, com netflix, com comida delivery, internet, casa própria, salário em dia " o choro é livre", mas que vende o almoço pra comprar a jantar, o choro não livre , ele é doloroso, ele é desesperador, e angustiante! fala tanto de empatia!</t>
+  </si>
+  <si>
+    <t>me falem uns filmes mt bons pra eu ver na netflix, amazon, disney+ e derivados pfff</t>
+  </si>
+  <si>
+    <t>cara esse filme q a netflix fez do death note é horrível</t>
+  </si>
+  <si>
+    <t>@rmp_joao @op_netflix_fan @purquegio este mano é o brabo</t>
+  </si>
+  <si>
+    <t>sim gente ele é o menino de peter punk e o menino que vai fazer rbd netflix https://t.co/ta7iywsjbm</t>
   </si>
   <si>
     <t>quero assistir tvd dnv af netflix pq me odeias</t>
   </si>
   <si>
-    <t>@standetudoh vai participar do rbd netflix</t>
-  </si>
-  <si>
-    <t>@luvkilluaz yaas é perfeito
-tem na netflix assisto logo</t>
-  </si>
-  <si>
-    <t>."estou assistindo a programas infantis com ela [khai] na tv e na netflix, aprendendo canções infantis, rolando com ela e apenas cantando para ela. é um ritmo de vida muito diferente, mas tem sido muito fácil de ajustar e isso é o mais surpreendente." - zayn</t>
-  </si>
-  <si>
-    <t>“netflix tax” à portuguesa, definição: legislar para conseguir taxar 2 ou 3 empresas, esquecendo a evolução do mercado e bloqueando desde logo o acesso a pmes. 
-😬
- https://t.co/6nuws2xpxa via @expresso https://t.co/sk0gqvgafg</t>
-  </si>
-  <si>
-    <t>alguém me indica uma série com uma temporada que tenha na globoplay, netflix ou prime video pra eu começar hoje</t>
-  </si>
-  <si>
-    <t>bruno gagliasso estreia 'santo', produção internacional da netflix.
-https://t.co/dn3bx42zbp https://t.co/au4krldy2c</t>
-  </si>
-  <si>
-    <t>não tem absolutamente uma pessoa que não seja insuportável dessa polos opostos da netflix, não sei porque continuo assistindo isso</t>
-  </si>
-  <si>
-    <t>esse lindo e amado anjo @kat_mcnamara é dona absoluta do meu coração #shadowhunters #saveshadowhunters #claryfairchild @constantinfilm @netflix @thecw https://t.co/v6f7okwad1</t>
-  </si>
-  <si>
-    <t>queria assistir friends mas nao tem mais friends na netflix wue vida triste</t>
-  </si>
-  <si>
-    <t>tiraram um maluco no pedaço da netflix eu vou cometer um crime</t>
-  </si>
-  <si>
-    <t>vamos todos juntos continuar lutando pela volta da nossa linda série, desistir jamais #shadowhunters #saveshadowhunters @constantinfilm @netflix @shadowhunterstv @thecw https://t.co/y6jzmtqejx</t>
-  </si>
-  <si>
-    <t>tava no tédio e achei na netflix
-we love you kyndra https://t.co/gmfqxsrhth</t>
-  </si>
-  <si>
-    <t>@antoniobaggio8 @lembrancaspv @landonorrisbr @netflix chefe de cozinha é questionável pq já deixou algumas vezes a comida queimar 😂😂😂</t>
-  </si>
-  <si>
-    <t>é fácil dizer isso, para quem vive numa bolha, salário em dia, geladeira cheia, um vinhozinho para relaxar à noite, vendo um filme na netflix.
-@majucoutinho https://t.co/8xoctngajb</t>
-  </si>
-  <si>
-    <t>@25o8s que demora agiliza netflix eu preciso ve com minha namorada</t>
-  </si>
-  <si>
-    <t>@_otakusbr talvez a netflix só coloque diu pq tem a ver com o rohan sla mas daí n tem graça</t>
-  </si>
-  <si>
-    <t>@lacastelleone_ a risque faz o papel dela enquanto netflix só decepciona</t>
-  </si>
-  <si>
-    <t>#netflix anuncia ‘santo’, série espanhola com bruno gagliasso e raúl arévalo. 
-a trama gira em torno de santo, um narcotraficante cujo rosto nunca foi visto e que é investigado pelos policiais federais. 
-‘santo’ ainda não tem data de lançamento. https://t.co/7kdusepnuk</t>
-  </si>
-  <si>
-    <t>@gicarmignani reza a lenda que tão remasterizando tudo em 4k pra sair na netflix!</t>
-  </si>
-  <si>
-    <t>sobre relacionamentos 
-1. não
-2. nenhuma
-3. touro
-4. quero muito
-5. apegado
-6. sim kkkk
-7. não/não sei 
-8. solteiro 😪
-9. os dois
-10. netflix em casa
-11. acredito em pessoas q se completam 
-12. não sei kkkkk
-13. claro
-curte q eu mando
-(as respostas podem ficar so na dm tb, haha)</t>
-  </si>
-  <si>
-    <t>@talitismo o livro é muito bom, e a série na netflix parece que será tão boa quanto!</t>
-  </si>
-  <si>
-    <t>netflix pague o meu tratamento psicológico agora depois desse final podre</t>
-  </si>
-  <si>
-    <t>por mim a gente já tava agarradinho procurando um filme na netflix</t>
-  </si>
-  <si>
-    <t>@weekndpink tô vendo o corte normal na netflix, mas já tem drive pelo tt do snyder cut vou assistir por drive https://t.co/92boyk6dtb</t>
-  </si>
-  <si>
-    <t>saiu a decima primeira temporada de modern family na netflix ovo chora</t>
-  </si>
-  <si>
-    <t>assistindo a saga crepúsculo pela 35x desde que entrou no catálogo da netflix</t>
-  </si>
-  <si>
-    <t>@netflixbrasil faz uma versão com o povo  branco que entra na uerj com cota para negros https://t.co/e1ndqkkbmc</t>
-  </si>
-  <si>
-    <t>procuro amigos p rachar esse netflix</t>
+    <t>@shinzoout https://t.co/7klohjlvwm
+se sua net aguenta uma netflix vai aguentar um torrent com seed razoável nisso aqui</t>
+  </si>
+  <si>
+    <t>@twolana9 netflix
+forças complex</t>
   </si>
   <si>
     <t>Teste</t>
-  </si>
-  <si>
-    <t>Classificação</t>
   </si>
 </sst>
 </file>
@@ -2248,13 +2239,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D304" sqref="D304"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C303" sqref="C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="183.109375" customWidth="1"/>
+    <col min="1" max="1" width="123.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3764,97 +3755,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:A202"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="173.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="73.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>314</v>
       </c>
@@ -4791,6 +4778,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>